<commit_message>
v6.6: new fifth wheel options
</commit_message>
<xml_diff>
--- a/adjustmentsRemote.xlsx
+++ b/adjustmentsRemote.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10914"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/MacData/Users/martinsommer/Documents/Programmieren/GitHub/RC/Rc_Engine_Sound_ESP32/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/martinsommer/Documents/Programmieren/GitHub/RC/Rc_Engine_Sound_ESP32/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9912A7E-D1A5-1E4E-A04E-F143FF72D0AE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3EC101E-8D65-3748-B7E4-9049196E76CB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2140" yWindow="1380" windowWidth="46720" windowHeight="24940" xr2:uid="{7FD8C6E5-3068-1C47-BC39-03FF60370E8F}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="101">
   <si>
     <t>up</t>
   </si>
@@ -235,29 +235,6 @@
   </si>
   <si>
     <t>Micro RC (WLTOYS pistol grip housing, connect it in SBUS communication mode)</t>
-  </si>
-  <si>
-    <r>
-      <t>5th wheel unlocking (</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri (Textkörper)_x0000_"/>
-      </rPr>
-      <t>res</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>)</t>
-    </r>
   </si>
   <si>
     <t>not available (Switch A internally used for DR)</t>
@@ -356,6 +333,9 @@
       </rPr>
       <t>If your assignment  is different, change the "Remote channel" accordingly in "adjustmentsRemote.h"</t>
     </r>
+  </si>
+  <si>
+    <t>5th wheel unlocking (3</t>
   </si>
   <si>
     <r>
@@ -407,13 +387,35 @@
       </rPr>
       <t>Note, that the PPM input was moved to the "RX" header</t>
     </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri (Textkörper)"/>
+      </rPr>
+      <t>NEVER connect servos to the CH headers in PWM mode</t>
+    </r>
+  </si>
+  <si>
+    <t>(3 = not in PWM communication mode. Connect servo to CH4 header</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -440,6 +442,11 @@
       <sz val="12"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri (Textkörper)_x0000_"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri (Textkörper)"/>
     </font>
   </fonts>
   <fills count="9">
@@ -492,7 +499,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -615,11 +622,82 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="65">
+  <cellXfs count="78">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -653,155 +731,194 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1172,7 +1289,7 @@
   <dimension ref="A1:U44"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="M44" sqref="M44"/>
+      <selection activeCell="J44" sqref="J44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1198,87 +1315,87 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21">
-      <c r="A1" s="44" t="s">
+      <c r="A1" s="27" t="s">
         <v>34</v>
       </c>
-      <c r="B1" s="44"/>
-      <c r="C1" s="44"/>
-      <c r="D1" s="44"/>
-      <c r="E1" s="44"/>
-      <c r="F1" s="44"/>
-      <c r="G1" s="45"/>
-      <c r="I1" s="20" t="s">
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
+      <c r="F1" s="27"/>
+      <c r="G1" s="28"/>
+      <c r="I1" s="58" t="s">
         <v>33</v>
       </c>
-      <c r="J1" s="20"/>
-      <c r="K1" s="20"/>
-      <c r="L1" s="20"/>
-      <c r="M1" s="20"/>
-      <c r="N1" s="20"/>
-      <c r="P1" s="32" t="s">
+      <c r="J1" s="58"/>
+      <c r="K1" s="58"/>
+      <c r="L1" s="58"/>
+      <c r="M1" s="58"/>
+      <c r="N1" s="58"/>
+      <c r="P1" s="56" t="s">
         <v>68</v>
       </c>
-      <c r="Q1" s="32"/>
-      <c r="R1" s="32"/>
-      <c r="S1" s="32"/>
-      <c r="T1" s="32"/>
-      <c r="U1" s="32"/>
+      <c r="Q1" s="56"/>
+      <c r="R1" s="56"/>
+      <c r="S1" s="56"/>
+      <c r="T1" s="56"/>
+      <c r="U1" s="56"/>
     </row>
     <row r="2" spans="1:21">
-      <c r="A2" s="43" t="s">
-        <v>87</v>
-      </c>
-      <c r="B2" s="43"/>
-      <c r="C2" s="43"/>
-      <c r="D2" s="43"/>
-      <c r="E2" s="23" t="s">
-        <v>72</v>
-      </c>
-      <c r="F2" s="21" t="s">
-        <v>78</v>
-      </c>
-      <c r="G2" s="23" t="s">
+      <c r="A2" s="26" t="s">
+        <v>86</v>
+      </c>
+      <c r="B2" s="26"/>
+      <c r="C2" s="26"/>
+      <c r="D2" s="26"/>
+      <c r="E2" s="24" t="s">
+        <v>71</v>
+      </c>
+      <c r="F2" s="59" t="s">
+        <v>77</v>
+      </c>
+      <c r="G2" s="24" t="s">
         <v>17</v>
       </c>
-      <c r="I2" s="31" t="s">
+      <c r="I2" s="57" t="s">
         <v>28</v>
       </c>
-      <c r="J2" s="31"/>
-      <c r="K2" s="31"/>
-      <c r="L2" s="31"/>
-      <c r="M2" s="31" t="s">
+      <c r="J2" s="57"/>
+      <c r="K2" s="57"/>
+      <c r="L2" s="57"/>
+      <c r="M2" s="57" t="s">
         <v>27</v>
       </c>
-      <c r="N2" s="31"/>
-      <c r="P2" s="31" t="s">
+      <c r="N2" s="57"/>
+      <c r="P2" s="57" t="s">
         <v>28</v>
       </c>
-      <c r="Q2" s="31"/>
-      <c r="R2" s="31"/>
-      <c r="S2" s="31"/>
-      <c r="T2" s="31" t="s">
+      <c r="Q2" s="57"/>
+      <c r="R2" s="57"/>
+      <c r="S2" s="57"/>
+      <c r="T2" s="57" t="s">
         <v>27</v>
       </c>
-      <c r="U2" s="31"/>
+      <c r="U2" s="57"/>
     </row>
     <row r="3" spans="1:21" ht="32" customHeight="1">
       <c r="A3" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="C3" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="D3" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="E3" s="24"/>
-      <c r="F3" s="22"/>
-      <c r="G3" s="24"/>
+      <c r="E3" s="25"/>
+      <c r="F3" s="60"/>
+      <c r="G3" s="25"/>
       <c r="I3" s="10" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="J3" s="2" t="s">
         <v>17</v>
@@ -1296,7 +1413,7 @@
         <v>26</v>
       </c>
       <c r="P3" s="10" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="Q3" s="2" t="s">
         <v>17</v>
@@ -1315,19 +1432,19 @@
       </c>
     </row>
     <row r="4" spans="1:21">
-      <c r="A4" s="46" t="s">
-        <v>80</v>
-      </c>
-      <c r="B4" s="46" t="s">
-        <v>88</v>
-      </c>
-      <c r="C4" s="46" t="s">
-        <v>77</v>
-      </c>
-      <c r="D4" s="46" t="s">
-        <v>88</v>
-      </c>
-      <c r="E4" s="36" t="s">
+      <c r="A4" s="29" t="s">
+        <v>79</v>
+      </c>
+      <c r="B4" s="29" t="s">
+        <v>87</v>
+      </c>
+      <c r="C4" s="29" t="s">
+        <v>76</v>
+      </c>
+      <c r="D4" s="29" t="s">
+        <v>87</v>
+      </c>
+      <c r="E4" s="39" t="s">
         <v>56</v>
       </c>
       <c r="F4" s="11">
@@ -1344,10 +1461,10 @@
       </c>
       <c r="K4" s="1"/>
       <c r="L4" s="1"/>
-      <c r="M4" s="15" t="s">
+      <c r="M4" s="38" t="s">
         <v>21</v>
       </c>
-      <c r="N4" s="15"/>
+      <c r="N4" s="38"/>
       <c r="P4" s="4">
         <v>1</v>
       </c>
@@ -1356,17 +1473,17 @@
       </c>
       <c r="R4" s="1"/>
       <c r="S4" s="1"/>
-      <c r="T4" s="15" t="s">
+      <c r="T4" s="38" t="s">
         <v>21</v>
       </c>
-      <c r="U4" s="15"/>
+      <c r="U4" s="38"/>
     </row>
     <row r="5" spans="1:21">
-      <c r="A5" s="46"/>
-      <c r="B5" s="46"/>
-      <c r="C5" s="46"/>
-      <c r="D5" s="46"/>
-      <c r="E5" s="36"/>
+      <c r="A5" s="29"/>
+      <c r="B5" s="29"/>
+      <c r="C5" s="29"/>
+      <c r="D5" s="29"/>
+      <c r="E5" s="39"/>
       <c r="F5" s="11">
         <v>2</v>
       </c>
@@ -1381,10 +1498,10 @@
       </c>
       <c r="K5" s="1"/>
       <c r="L5" s="1"/>
-      <c r="M5" s="15" t="s">
+      <c r="M5" s="38" t="s">
         <v>39</v>
       </c>
-      <c r="N5" s="15"/>
+      <c r="N5" s="38"/>
       <c r="P5" s="4">
         <v>2</v>
       </c>
@@ -1393,17 +1510,17 @@
       </c>
       <c r="R5" s="1"/>
       <c r="S5" s="1"/>
-      <c r="T5" s="15" t="s">
+      <c r="T5" s="38" t="s">
         <v>39</v>
       </c>
-      <c r="U5" s="15"/>
+      <c r="U5" s="38"/>
     </row>
     <row r="6" spans="1:21">
-      <c r="A6" s="46"/>
-      <c r="B6" s="46"/>
-      <c r="C6" s="46"/>
-      <c r="D6" s="46"/>
-      <c r="E6" s="36"/>
+      <c r="A6" s="29"/>
+      <c r="B6" s="29"/>
+      <c r="C6" s="29"/>
+      <c r="D6" s="29"/>
+      <c r="E6" s="39"/>
       <c r="F6" s="11">
         <v>3</v>
       </c>
@@ -1418,10 +1535,10 @@
       </c>
       <c r="K6" s="1"/>
       <c r="L6" s="1"/>
-      <c r="M6" s="15" t="s">
+      <c r="M6" s="38" t="s">
         <v>23</v>
       </c>
-      <c r="N6" s="15"/>
+      <c r="N6" s="38"/>
       <c r="P6" s="4">
         <v>3</v>
       </c>
@@ -1430,17 +1547,17 @@
       </c>
       <c r="R6" s="1"/>
       <c r="S6" s="1"/>
-      <c r="T6" s="15" t="s">
+      <c r="T6" s="38" t="s">
         <v>23</v>
       </c>
-      <c r="U6" s="15"/>
+      <c r="U6" s="38"/>
     </row>
     <row r="7" spans="1:21">
-      <c r="A7" s="46"/>
-      <c r="B7" s="46"/>
-      <c r="C7" s="46"/>
-      <c r="D7" s="46"/>
-      <c r="E7" s="36"/>
+      <c r="A7" s="29"/>
+      <c r="B7" s="29"/>
+      <c r="C7" s="29"/>
+      <c r="D7" s="29"/>
+      <c r="E7" s="39"/>
       <c r="F7" s="11">
         <v>4</v>
       </c>
@@ -1455,10 +1572,10 @@
       </c>
       <c r="K7" s="1"/>
       <c r="L7" s="1"/>
-      <c r="M7" s="15" t="s">
+      <c r="M7" s="38" t="s">
         <v>41</v>
       </c>
-      <c r="N7" s="15"/>
+      <c r="N7" s="38"/>
       <c r="P7" s="4">
         <v>5</v>
       </c>
@@ -1467,30 +1584,30 @@
       </c>
       <c r="R7" s="1"/>
       <c r="S7" s="1"/>
-      <c r="T7" s="15" t="s">
+      <c r="T7" s="38" t="s">
         <v>41</v>
       </c>
-      <c r="U7" s="15"/>
+      <c r="U7" s="38"/>
     </row>
     <row r="8" spans="1:21">
-      <c r="A8" s="46"/>
-      <c r="B8" s="46"/>
-      <c r="C8" s="46"/>
-      <c r="D8" s="46"/>
-      <c r="E8" s="36"/>
-      <c r="F8" s="25">
+      <c r="A8" s="29"/>
+      <c r="B8" s="29"/>
+      <c r="C8" s="29"/>
+      <c r="D8" s="29"/>
+      <c r="E8" s="39"/>
+      <c r="F8" s="61">
         <v>5</v>
       </c>
-      <c r="G8" s="28" t="s">
+      <c r="G8" s="53" t="s">
         <v>36</v>
       </c>
-      <c r="I8" s="17">
+      <c r="I8" s="47">
         <v>2</v>
       </c>
-      <c r="J8" s="59" t="s">
+      <c r="J8" s="48" t="s">
         <v>19</v>
       </c>
-      <c r="K8" s="18" t="s">
+      <c r="K8" s="51" t="s">
         <v>0</v>
       </c>
       <c r="L8" s="1" t="s">
@@ -1502,13 +1619,13 @@
       <c r="N8" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="P8" s="17">
+      <c r="P8" s="47">
         <v>4</v>
       </c>
-      <c r="Q8" s="59" t="s">
-        <v>84</v>
-      </c>
-      <c r="R8" s="18" t="s">
+      <c r="Q8" s="48" t="s">
+        <v>83</v>
+      </c>
+      <c r="R8" s="51" t="s">
         <v>12</v>
       </c>
       <c r="S8" s="1" t="s">
@@ -1522,169 +1639,169 @@
       </c>
     </row>
     <row r="9" spans="1:21">
-      <c r="A9" s="46"/>
-      <c r="B9" s="46"/>
-      <c r="C9" s="46"/>
-      <c r="D9" s="46"/>
-      <c r="E9" s="36"/>
-      <c r="F9" s="26"/>
-      <c r="G9" s="29"/>
-      <c r="I9" s="17"/>
-      <c r="J9" s="60"/>
-      <c r="K9" s="18"/>
+      <c r="A9" s="29"/>
+      <c r="B9" s="29"/>
+      <c r="C9" s="29"/>
+      <c r="D9" s="29"/>
+      <c r="E9" s="39"/>
+      <c r="F9" s="62"/>
+      <c r="G9" s="54"/>
+      <c r="I9" s="47"/>
+      <c r="J9" s="49"/>
+      <c r="K9" s="51"/>
       <c r="L9" s="1" t="s">
         <v>6</v>
       </c>
       <c r="M9" s="1"/>
-      <c r="N9" s="19"/>
-      <c r="P9" s="17"/>
-      <c r="Q9" s="60"/>
-      <c r="R9" s="18"/>
+      <c r="N9" s="52"/>
+      <c r="P9" s="47"/>
+      <c r="Q9" s="49"/>
+      <c r="R9" s="51"/>
       <c r="S9" s="1" t="s">
         <v>6</v>
       </c>
       <c r="T9" s="1"/>
-      <c r="U9" s="19"/>
+      <c r="U9" s="52"/>
     </row>
     <row r="10" spans="1:21">
-      <c r="A10" s="46"/>
-      <c r="B10" s="46"/>
-      <c r="C10" s="46"/>
-      <c r="D10" s="46"/>
-      <c r="E10" s="36"/>
-      <c r="F10" s="26"/>
-      <c r="G10" s="29"/>
-      <c r="I10" s="17"/>
-      <c r="J10" s="60"/>
-      <c r="K10" s="18"/>
+      <c r="A10" s="29"/>
+      <c r="B10" s="29"/>
+      <c r="C10" s="29"/>
+      <c r="D10" s="29"/>
+      <c r="E10" s="39"/>
+      <c r="F10" s="62"/>
+      <c r="G10" s="54"/>
+      <c r="I10" s="47"/>
+      <c r="J10" s="49"/>
+      <c r="K10" s="51"/>
       <c r="L10" s="1" t="s">
         <v>7</v>
       </c>
       <c r="M10" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="N10" s="19"/>
-      <c r="P10" s="17"/>
-      <c r="Q10" s="60"/>
-      <c r="R10" s="18"/>
+      <c r="N10" s="52"/>
+      <c r="P10" s="47"/>
+      <c r="Q10" s="49"/>
+      <c r="R10" s="51"/>
       <c r="S10" s="1" t="s">
         <v>7</v>
       </c>
       <c r="T10" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="U10" s="19"/>
+      <c r="U10" s="52"/>
     </row>
     <row r="11" spans="1:21">
-      <c r="A11" s="46"/>
-      <c r="B11" s="46"/>
-      <c r="C11" s="46"/>
-      <c r="D11" s="46"/>
-      <c r="E11" s="36"/>
-      <c r="F11" s="26"/>
-      <c r="G11" s="29"/>
-      <c r="I11" s="17"/>
-      <c r="J11" s="60"/>
-      <c r="K11" s="18" t="s">
+      <c r="A11" s="29"/>
+      <c r="B11" s="29"/>
+      <c r="C11" s="29"/>
+      <c r="D11" s="29"/>
+      <c r="E11" s="39"/>
+      <c r="F11" s="62"/>
+      <c r="G11" s="54"/>
+      <c r="I11" s="47"/>
+      <c r="J11" s="49"/>
+      <c r="K11" s="51" t="s">
         <v>1</v>
       </c>
       <c r="L11" s="1" t="s">
         <v>5</v>
       </c>
       <c r="M11" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="N11" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="P11" s="17"/>
-      <c r="Q11" s="60"/>
-      <c r="R11" s="18" t="s">
+      <c r="P11" s="47"/>
+      <c r="Q11" s="49"/>
+      <c r="R11" s="51" t="s">
         <v>13</v>
       </c>
       <c r="S11" s="1" t="s">
         <v>5</v>
       </c>
       <c r="T11" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="U11" s="8" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="12" spans="1:21">
-      <c r="A12" s="46"/>
-      <c r="B12" s="46"/>
-      <c r="C12" s="46"/>
-      <c r="D12" s="46"/>
-      <c r="E12" s="36"/>
-      <c r="F12" s="26"/>
-      <c r="G12" s="29"/>
-      <c r="I12" s="17"/>
-      <c r="J12" s="60"/>
-      <c r="K12" s="18"/>
+      <c r="A12" s="29"/>
+      <c r="B12" s="29"/>
+      <c r="C12" s="29"/>
+      <c r="D12" s="29"/>
+      <c r="E12" s="39"/>
+      <c r="F12" s="62"/>
+      <c r="G12" s="54"/>
+      <c r="I12" s="47"/>
+      <c r="J12" s="49"/>
+      <c r="K12" s="51"/>
       <c r="L12" s="1" t="s">
         <v>6</v>
       </c>
       <c r="M12" s="1"/>
-      <c r="N12" s="19"/>
-      <c r="P12" s="17"/>
-      <c r="Q12" s="60"/>
-      <c r="R12" s="18"/>
+      <c r="N12" s="52"/>
+      <c r="P12" s="47"/>
+      <c r="Q12" s="49"/>
+      <c r="R12" s="51"/>
       <c r="S12" s="1" t="s">
         <v>6</v>
       </c>
       <c r="T12" s="1"/>
-      <c r="U12" s="19"/>
+      <c r="U12" s="52"/>
     </row>
     <row r="13" spans="1:21">
-      <c r="A13" s="46"/>
-      <c r="B13" s="46"/>
-      <c r="C13" s="46"/>
-      <c r="D13" s="46"/>
-      <c r="E13" s="36"/>
-      <c r="F13" s="27"/>
-      <c r="G13" s="30"/>
-      <c r="I13" s="17"/>
-      <c r="J13" s="61"/>
-      <c r="K13" s="18"/>
+      <c r="A13" s="29"/>
+      <c r="B13" s="29"/>
+      <c r="C13" s="29"/>
+      <c r="D13" s="29"/>
+      <c r="E13" s="39"/>
+      <c r="F13" s="63"/>
+      <c r="G13" s="55"/>
+      <c r="I13" s="47"/>
+      <c r="J13" s="50"/>
+      <c r="K13" s="51"/>
       <c r="L13" s="1" t="s">
         <v>7</v>
       </c>
       <c r="M13" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="N13" s="19"/>
-      <c r="P13" s="17"/>
-      <c r="Q13" s="61"/>
-      <c r="R13" s="18"/>
+      <c r="N13" s="52"/>
+      <c r="P13" s="47"/>
+      <c r="Q13" s="50"/>
+      <c r="R13" s="51"/>
       <c r="S13" s="1" t="s">
         <v>7</v>
       </c>
       <c r="T13" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="U13" s="19"/>
+      <c r="U13" s="52"/>
     </row>
     <row r="14" spans="1:21">
-      <c r="A14" s="46"/>
-      <c r="B14" s="46"/>
-      <c r="C14" s="46"/>
-      <c r="D14" s="46"/>
-      <c r="E14" s="36"/>
-      <c r="F14" s="25">
+      <c r="A14" s="29"/>
+      <c r="B14" s="29"/>
+      <c r="C14" s="29"/>
+      <c r="D14" s="29"/>
+      <c r="E14" s="39"/>
+      <c r="F14" s="61">
         <v>6</v>
       </c>
-      <c r="G14" s="28" t="s">
+      <c r="G14" s="53" t="s">
         <v>37</v>
       </c>
-      <c r="I14" s="17">
+      <c r="I14" s="47">
         <v>4</v>
       </c>
-      <c r="J14" s="59" t="s">
+      <c r="J14" s="48" t="s">
         <v>20</v>
       </c>
-      <c r="K14" s="18" t="s">
+      <c r="K14" s="51" t="s">
         <v>12</v>
       </c>
       <c r="L14" s="1" t="s">
@@ -1694,11 +1811,11 @@
       <c r="N14" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P14" s="39">
+      <c r="P14" s="42">
         <v>16</v>
       </c>
-      <c r="Q14" s="62"/>
-      <c r="R14" s="39"/>
+      <c r="Q14" s="43"/>
+      <c r="R14" s="42"/>
       <c r="S14" s="6" t="s">
         <v>5</v>
       </c>
@@ -1706,68 +1823,68 @@
       <c r="U14" s="6"/>
     </row>
     <row r="15" spans="1:21">
-      <c r="A15" s="46"/>
-      <c r="B15" s="46"/>
-      <c r="C15" s="46"/>
-      <c r="D15" s="46"/>
-      <c r="E15" s="36"/>
-      <c r="F15" s="26"/>
-      <c r="G15" s="29"/>
-      <c r="I15" s="17"/>
-      <c r="J15" s="60"/>
-      <c r="K15" s="18"/>
+      <c r="A15" s="29"/>
+      <c r="B15" s="29"/>
+      <c r="C15" s="29"/>
+      <c r="D15" s="29"/>
+      <c r="E15" s="39"/>
+      <c r="F15" s="62"/>
+      <c r="G15" s="54"/>
+      <c r="I15" s="47"/>
+      <c r="J15" s="49"/>
+      <c r="K15" s="51"/>
       <c r="L15" s="1" t="s">
         <v>6</v>
       </c>
       <c r="M15" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="N15" s="19"/>
-      <c r="P15" s="39"/>
-      <c r="Q15" s="63"/>
-      <c r="R15" s="39"/>
+      <c r="N15" s="52"/>
+      <c r="P15" s="42"/>
+      <c r="Q15" s="44"/>
+      <c r="R15" s="42"/>
       <c r="S15" s="6" t="s">
         <v>6</v>
       </c>
       <c r="T15" s="6"/>
-      <c r="U15" s="40"/>
+      <c r="U15" s="46"/>
     </row>
     <row r="16" spans="1:21">
-      <c r="A16" s="46"/>
-      <c r="B16" s="46"/>
-      <c r="C16" s="46"/>
-      <c r="D16" s="46"/>
-      <c r="E16" s="36"/>
-      <c r="F16" s="26"/>
-      <c r="G16" s="29"/>
-      <c r="I16" s="17"/>
-      <c r="J16" s="60"/>
-      <c r="K16" s="18"/>
+      <c r="A16" s="29"/>
+      <c r="B16" s="29"/>
+      <c r="C16" s="29"/>
+      <c r="D16" s="29"/>
+      <c r="E16" s="39"/>
+      <c r="F16" s="62"/>
+      <c r="G16" s="54"/>
+      <c r="I16" s="47"/>
+      <c r="J16" s="49"/>
+      <c r="K16" s="51"/>
       <c r="L16" s="1" t="s">
         <v>7</v>
       </c>
       <c r="M16" s="1"/>
-      <c r="N16" s="19"/>
-      <c r="P16" s="39"/>
-      <c r="Q16" s="63"/>
-      <c r="R16" s="39"/>
+      <c r="N16" s="52"/>
+      <c r="P16" s="42"/>
+      <c r="Q16" s="44"/>
+      <c r="R16" s="42"/>
       <c r="S16" s="6" t="s">
         <v>7</v>
       </c>
       <c r="T16" s="6"/>
-      <c r="U16" s="40"/>
+      <c r="U16" s="46"/>
     </row>
     <row r="17" spans="1:21">
-      <c r="A17" s="46"/>
-      <c r="B17" s="46"/>
-      <c r="C17" s="46"/>
-      <c r="D17" s="46"/>
-      <c r="E17" s="36"/>
-      <c r="F17" s="26"/>
-      <c r="G17" s="29"/>
-      <c r="I17" s="17"/>
-      <c r="J17" s="60"/>
-      <c r="K17" s="18" t="s">
+      <c r="A17" s="29"/>
+      <c r="B17" s="29"/>
+      <c r="C17" s="29"/>
+      <c r="D17" s="29"/>
+      <c r="E17" s="39"/>
+      <c r="F17" s="62"/>
+      <c r="G17" s="54"/>
+      <c r="I17" s="47"/>
+      <c r="J17" s="49"/>
+      <c r="K17" s="51" t="s">
         <v>13</v>
       </c>
       <c r="L17" s="1" t="s">
@@ -1775,11 +1892,11 @@
       </c>
       <c r="M17" s="1"/>
       <c r="N17" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="P17" s="39"/>
-      <c r="Q17" s="63"/>
-      <c r="R17" s="39"/>
+        <v>98</v>
+      </c>
+      <c r="P17" s="42"/>
+      <c r="Q17" s="44"/>
+      <c r="R17" s="42"/>
       <c r="S17" s="6" t="s">
         <v>5</v>
       </c>
@@ -1787,70 +1904,70 @@
       <c r="U17" s="6"/>
     </row>
     <row r="18" spans="1:21">
-      <c r="A18" s="46"/>
-      <c r="B18" s="46"/>
-      <c r="C18" s="46"/>
-      <c r="D18" s="46"/>
-      <c r="E18" s="36"/>
-      <c r="F18" s="26"/>
-      <c r="G18" s="29"/>
-      <c r="I18" s="17"/>
-      <c r="J18" s="60"/>
-      <c r="K18" s="18"/>
+      <c r="A18" s="29"/>
+      <c r="B18" s="29"/>
+      <c r="C18" s="29"/>
+      <c r="D18" s="29"/>
+      <c r="E18" s="39"/>
+      <c r="F18" s="62"/>
+      <c r="G18" s="54"/>
+      <c r="I18" s="47"/>
+      <c r="J18" s="49"/>
+      <c r="K18" s="51"/>
       <c r="L18" s="1" t="s">
         <v>6</v>
       </c>
       <c r="M18" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="N18" s="19"/>
-      <c r="P18" s="39"/>
-      <c r="Q18" s="63"/>
-      <c r="R18" s="39"/>
+      <c r="N18" s="52"/>
+      <c r="P18" s="42"/>
+      <c r="Q18" s="44"/>
+      <c r="R18" s="42"/>
       <c r="S18" s="6" t="s">
         <v>6</v>
       </c>
       <c r="T18" s="6"/>
-      <c r="U18" s="40"/>
+      <c r="U18" s="46"/>
     </row>
     <row r="19" spans="1:21">
-      <c r="A19" s="46"/>
-      <c r="B19" s="46"/>
-      <c r="C19" s="46"/>
-      <c r="D19" s="46"/>
-      <c r="E19" s="36"/>
-      <c r="F19" s="27"/>
-      <c r="G19" s="30"/>
-      <c r="I19" s="17"/>
-      <c r="J19" s="61"/>
-      <c r="K19" s="18"/>
+      <c r="A19" s="29"/>
+      <c r="B19" s="29"/>
+      <c r="C19" s="29"/>
+      <c r="D19" s="29"/>
+      <c r="E19" s="39"/>
+      <c r="F19" s="63"/>
+      <c r="G19" s="55"/>
+      <c r="I19" s="47"/>
+      <c r="J19" s="50"/>
+      <c r="K19" s="51"/>
       <c r="L19" s="1" t="s">
         <v>7</v>
       </c>
       <c r="M19" s="1"/>
-      <c r="N19" s="19"/>
-      <c r="P19" s="39"/>
-      <c r="Q19" s="64"/>
-      <c r="R19" s="39"/>
+      <c r="N19" s="52"/>
+      <c r="P19" s="42"/>
+      <c r="Q19" s="45"/>
+      <c r="R19" s="42"/>
       <c r="S19" s="6" t="s">
         <v>7</v>
       </c>
       <c r="T19" s="6"/>
-      <c r="U19" s="40"/>
+      <c r="U19" s="46"/>
     </row>
     <row r="20" spans="1:21">
-      <c r="A20" s="47" t="s">
-        <v>89</v>
-      </c>
-      <c r="B20" s="46"/>
-      <c r="C20" s="46"/>
-      <c r="D20" s="46"/>
-      <c r="E20" s="36"/>
+      <c r="A20" s="30" t="s">
+        <v>88</v>
+      </c>
+      <c r="B20" s="29"/>
+      <c r="C20" s="29"/>
+      <c r="D20" s="29"/>
+      <c r="E20" s="39"/>
       <c r="F20" s="11">
         <v>7</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="I20" s="4">
         <v>8</v>
@@ -1860,27 +1977,27 @@
       </c>
       <c r="K20" s="1"/>
       <c r="L20" s="1"/>
-      <c r="M20" s="16" t="s">
-        <v>91</v>
-      </c>
-      <c r="N20" s="16"/>
+      <c r="M20" s="64" t="s">
+        <v>90</v>
+      </c>
+      <c r="N20" s="64"/>
       <c r="P20" s="7">
         <v>16</v>
       </c>
       <c r="Q20" s="6"/>
       <c r="R20" s="6"/>
       <c r="S20" s="6"/>
-      <c r="T20" s="33" t="s">
+      <c r="T20" s="15" t="s">
         <v>45</v>
       </c>
-      <c r="U20" s="33"/>
+      <c r="U20" s="15"/>
     </row>
     <row r="21" spans="1:21" ht="16" customHeight="1">
-      <c r="A21" s="48"/>
-      <c r="B21" s="46"/>
-      <c r="C21" s="46"/>
-      <c r="D21" s="46"/>
-      <c r="E21" s="37" t="s">
+      <c r="A21" s="31"/>
+      <c r="B21" s="29"/>
+      <c r="C21" s="29"/>
+      <c r="D21" s="29"/>
+      <c r="E21" s="40" t="s">
         <v>59</v>
       </c>
       <c r="F21" s="11">
@@ -1897,10 +2014,10 @@
       </c>
       <c r="K21" s="1"/>
       <c r="L21" s="1"/>
-      <c r="M21" s="15" t="s">
-        <v>96</v>
-      </c>
-      <c r="N21" s="15"/>
+      <c r="M21" s="38" t="s">
+        <v>95</v>
+      </c>
+      <c r="N21" s="38"/>
       <c r="P21" s="4">
         <v>6</v>
       </c>
@@ -1909,19 +2026,19 @@
       </c>
       <c r="R21" s="1"/>
       <c r="S21" s="1"/>
-      <c r="T21" s="15" t="s">
-        <v>96</v>
-      </c>
-      <c r="U21" s="15"/>
+      <c r="T21" s="38" t="s">
+        <v>95</v>
+      </c>
+      <c r="U21" s="38"/>
     </row>
     <row r="22" spans="1:21">
-      <c r="A22" s="48"/>
-      <c r="B22" s="47" t="s">
-        <v>89</v>
-      </c>
-      <c r="C22" s="46"/>
-      <c r="D22" s="46"/>
-      <c r="E22" s="38"/>
+      <c r="A22" s="31"/>
+      <c r="B22" s="30" t="s">
+        <v>88</v>
+      </c>
+      <c r="C22" s="29"/>
+      <c r="D22" s="29"/>
+      <c r="E22" s="41"/>
       <c r="F22" s="11">
         <v>9</v>
       </c>
@@ -1936,10 +2053,10 @@
       </c>
       <c r="K22" s="1"/>
       <c r="L22" s="1"/>
-      <c r="M22" s="34" t="s">
-        <v>92</v>
-      </c>
-      <c r="N22" s="35"/>
+      <c r="M22" s="16" t="s">
+        <v>91</v>
+      </c>
+      <c r="N22" s="17"/>
       <c r="P22" s="4">
         <v>7</v>
       </c>
@@ -1948,16 +2065,16 @@
       </c>
       <c r="R22" s="1"/>
       <c r="S22" s="1"/>
-      <c r="T22" s="34" t="s">
-        <v>92</v>
-      </c>
-      <c r="U22" s="35"/>
+      <c r="T22" s="16" t="s">
+        <v>91</v>
+      </c>
+      <c r="U22" s="17"/>
     </row>
     <row r="23" spans="1:21" ht="17">
-      <c r="A23" s="48"/>
-      <c r="B23" s="48"/>
-      <c r="C23" s="46"/>
-      <c r="D23" s="46"/>
+      <c r="A23" s="31"/>
+      <c r="B23" s="31"/>
+      <c r="C23" s="29"/>
+      <c r="D23" s="29"/>
       <c r="E23" s="12" t="s">
         <v>7</v>
       </c>
@@ -1973,10 +2090,10 @@
       <c r="J23" s="6"/>
       <c r="K23" s="6"/>
       <c r="L23" s="6"/>
-      <c r="M23" s="33" t="s">
-        <v>70</v>
-      </c>
-      <c r="N23" s="33"/>
+      <c r="M23" s="15" t="s">
+        <v>69</v>
+      </c>
+      <c r="N23" s="15"/>
       <c r="P23" s="4">
         <v>8</v>
       </c>
@@ -1985,17 +2102,17 @@
       </c>
       <c r="R23" s="1"/>
       <c r="S23" s="1"/>
-      <c r="T23" s="34" t="s">
+      <c r="T23" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="U23" s="35"/>
+      <c r="U23" s="17"/>
     </row>
     <row r="24" spans="1:21">
-      <c r="A24" s="48"/>
-      <c r="B24" s="48"/>
-      <c r="C24" s="46"/>
-      <c r="D24" s="46"/>
-      <c r="E24" s="50" t="s">
+      <c r="A24" s="31"/>
+      <c r="B24" s="31"/>
+      <c r="C24" s="29"/>
+      <c r="D24" s="29"/>
+      <c r="E24" s="33" t="s">
         <v>57</v>
       </c>
       <c r="F24" s="11">
@@ -2010,10 +2127,10 @@
       <c r="J24" s="6"/>
       <c r="K24" s="6"/>
       <c r="L24" s="6"/>
-      <c r="M24" s="33" t="s">
+      <c r="M24" s="15" t="s">
         <v>45</v>
       </c>
-      <c r="N24" s="33"/>
+      <c r="N24" s="15"/>
       <c r="P24" s="4">
         <v>9</v>
       </c>
@@ -2022,17 +2139,17 @@
       </c>
       <c r="R24" s="1"/>
       <c r="S24" s="1"/>
-      <c r="T24" s="34" t="s">
+      <c r="T24" s="16" t="s">
         <v>60</v>
       </c>
-      <c r="U24" s="35"/>
+      <c r="U24" s="17"/>
     </row>
     <row r="25" spans="1:21">
-      <c r="A25" s="48"/>
-      <c r="B25" s="48"/>
-      <c r="C25" s="46"/>
-      <c r="D25" s="46"/>
-      <c r="E25" s="51"/>
+      <c r="A25" s="31"/>
+      <c r="B25" s="31"/>
+      <c r="C25" s="29"/>
+      <c r="D25" s="29"/>
+      <c r="E25" s="34"/>
       <c r="F25" s="11">
         <v>12</v>
       </c>
@@ -2045,10 +2162,10 @@
       <c r="J25" s="6"/>
       <c r="K25" s="6"/>
       <c r="L25" s="6"/>
-      <c r="M25" s="33" t="s">
+      <c r="M25" s="15" t="s">
         <v>45</v>
       </c>
-      <c r="N25" s="33"/>
+      <c r="N25" s="15"/>
       <c r="P25" s="4">
         <v>10</v>
       </c>
@@ -2057,17 +2174,17 @@
       </c>
       <c r="R25" s="1"/>
       <c r="S25" s="1"/>
-      <c r="T25" s="41" t="s">
+      <c r="T25" s="36" t="s">
         <v>62</v>
       </c>
-      <c r="U25" s="42"/>
+      <c r="U25" s="37"/>
     </row>
     <row r="26" spans="1:21">
-      <c r="A26" s="49"/>
-      <c r="B26" s="48"/>
-      <c r="C26" s="46"/>
-      <c r="D26" s="46"/>
-      <c r="E26" s="52"/>
+      <c r="A26" s="32"/>
+      <c r="B26" s="31"/>
+      <c r="C26" s="29"/>
+      <c r="D26" s="29"/>
+      <c r="E26" s="35"/>
       <c r="F26" s="11">
         <v>13</v>
       </c>
@@ -2080,10 +2197,10 @@
       <c r="J26" s="6"/>
       <c r="K26" s="6"/>
       <c r="L26" s="6"/>
-      <c r="M26" s="33" t="s">
+      <c r="M26" s="15" t="s">
         <v>45</v>
       </c>
-      <c r="N26" s="33"/>
+      <c r="N26" s="15"/>
       <c r="P26" s="4">
         <v>11</v>
       </c>
@@ -2092,200 +2209,208 @@
       </c>
       <c r="R26" s="1"/>
       <c r="S26" s="1"/>
-      <c r="T26" s="41" t="s">
+      <c r="T26" s="36" t="s">
         <v>63</v>
       </c>
-      <c r="U26" s="42"/>
+      <c r="U26" s="37"/>
     </row>
     <row r="28" spans="1:21">
-      <c r="A28" s="55" t="s">
+      <c r="A28" s="20" t="s">
+        <v>81</v>
+      </c>
+      <c r="B28" s="20"/>
+      <c r="C28" s="20"/>
+      <c r="D28" s="20"/>
+      <c r="E28" s="20"/>
+      <c r="F28" s="20"/>
+      <c r="G28" s="20"/>
+      <c r="I28" s="19" t="s">
+        <v>70</v>
+      </c>
+      <c r="J28" s="19"/>
+      <c r="K28" s="19"/>
+      <c r="L28" s="19"/>
+      <c r="M28" s="19"/>
+      <c r="N28" s="19"/>
+      <c r="P28" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="29" spans="1:21">
+      <c r="A29" s="21" t="s">
+        <v>80</v>
+      </c>
+      <c r="B29" s="21"/>
+      <c r="C29" s="21"/>
+      <c r="D29" s="21"/>
+      <c r="E29" s="21"/>
+      <c r="F29" s="21"/>
+      <c r="G29" s="21"/>
+      <c r="I29" s="18" t="s">
         <v>82</v>
       </c>
-      <c r="B28" s="55"/>
-      <c r="C28" s="55"/>
-      <c r="D28" s="55"/>
-      <c r="E28" s="55"/>
-      <c r="F28" s="55"/>
-      <c r="G28" s="55"/>
-      <c r="I28" s="54" t="s">
-        <v>71</v>
-      </c>
-      <c r="J28" s="54"/>
-      <c r="K28" s="54"/>
-      <c r="L28" s="54"/>
-      <c r="M28" s="54"/>
-      <c r="N28" s="54"/>
-      <c r="P28" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="29" spans="1:21">
-      <c r="A29" s="56" t="s">
-        <v>81</v>
-      </c>
-      <c r="B29" s="56"/>
-      <c r="C29" s="56"/>
-      <c r="D29" s="56"/>
-      <c r="E29" s="56"/>
-      <c r="F29" s="56"/>
-      <c r="G29" s="56"/>
-      <c r="I29" s="53" t="s">
-        <v>83</v>
-      </c>
-      <c r="J29" s="54"/>
-      <c r="K29" s="54"/>
-      <c r="L29" s="54"/>
-      <c r="M29" s="54"/>
-      <c r="N29" s="54"/>
+      <c r="J29" s="19"/>
+      <c r="K29" s="19"/>
+      <c r="L29" s="19"/>
+      <c r="M29" s="19"/>
+      <c r="N29" s="19"/>
     </row>
     <row r="30" spans="1:21">
-      <c r="A30" s="57" t="s">
-        <v>93</v>
-      </c>
-      <c r="B30" s="57"/>
-      <c r="C30" s="57"/>
-      <c r="D30" s="57"/>
-      <c r="E30" s="57"/>
-      <c r="F30" s="57"/>
-      <c r="G30" s="57"/>
-      <c r="I30" s="54"/>
-      <c r="J30" s="54"/>
-      <c r="K30" s="54"/>
-      <c r="L30" s="54"/>
-      <c r="M30" s="54"/>
-      <c r="N30" s="54"/>
+      <c r="A30" s="22" t="s">
+        <v>92</v>
+      </c>
+      <c r="B30" s="22"/>
+      <c r="C30" s="22"/>
+      <c r="D30" s="22"/>
+      <c r="E30" s="22"/>
+      <c r="F30" s="22"/>
+      <c r="G30" s="22"/>
+      <c r="I30" s="19"/>
+      <c r="J30" s="19"/>
+      <c r="K30" s="19"/>
+      <c r="L30" s="19"/>
+      <c r="M30" s="19"/>
+      <c r="N30" s="19"/>
     </row>
     <row r="31" spans="1:21" ht="16" customHeight="1">
-      <c r="I31" s="58" t="s">
-        <v>98</v>
-      </c>
-      <c r="J31" s="58"/>
-      <c r="K31" s="58"/>
-      <c r="L31" s="58"/>
-      <c r="M31" s="58"/>
-      <c r="N31" s="58"/>
+      <c r="I31" s="23" t="s">
+        <v>97</v>
+      </c>
+      <c r="J31" s="23"/>
+      <c r="K31" s="23"/>
+      <c r="L31" s="23"/>
+      <c r="M31" s="23"/>
+      <c r="N31" s="23"/>
     </row>
     <row r="32" spans="1:21" ht="16" customHeight="1">
-      <c r="A32" s="58" t="s">
+      <c r="A32" s="71" t="s">
         <v>99</v>
       </c>
-      <c r="B32" s="58"/>
-      <c r="C32" s="58"/>
-      <c r="D32" s="58"/>
-      <c r="E32" s="58"/>
-      <c r="F32" s="58"/>
-      <c r="G32" s="58"/>
-      <c r="I32" s="58"/>
-      <c r="J32" s="58"/>
-      <c r="K32" s="58"/>
-      <c r="L32" s="58"/>
-      <c r="M32" s="58"/>
-      <c r="N32" s="58"/>
+      <c r="B32" s="69"/>
+      <c r="C32" s="69"/>
+      <c r="D32" s="69"/>
+      <c r="E32" s="69"/>
+      <c r="F32" s="69"/>
+      <c r="G32" s="72"/>
+      <c r="I32" s="23"/>
+      <c r="J32" s="23"/>
+      <c r="K32" s="23"/>
+      <c r="L32" s="23"/>
+      <c r="M32" s="23"/>
+      <c r="N32" s="23"/>
     </row>
     <row r="33" spans="1:14" ht="16" customHeight="1">
-      <c r="A33" s="58"/>
-      <c r="B33" s="58"/>
-      <c r="C33" s="58"/>
-      <c r="D33" s="58"/>
-      <c r="E33" s="58"/>
-      <c r="F33" s="58"/>
-      <c r="G33" s="58"/>
-      <c r="I33" s="58"/>
-      <c r="J33" s="58"/>
-      <c r="K33" s="58"/>
-      <c r="L33" s="58"/>
-      <c r="M33" s="58"/>
-      <c r="N33" s="58"/>
+      <c r="A33" s="73"/>
+      <c r="B33" s="70"/>
+      <c r="C33" s="70"/>
+      <c r="D33" s="70"/>
+      <c r="E33" s="70"/>
+      <c r="F33" s="70"/>
+      <c r="G33" s="74"/>
+      <c r="I33" s="23"/>
+      <c r="J33" s="23"/>
+      <c r="K33" s="23"/>
+      <c r="L33" s="23"/>
+      <c r="M33" s="23"/>
+      <c r="N33" s="23"/>
     </row>
     <row r="34" spans="1:14" ht="16" customHeight="1">
-      <c r="A34" s="58"/>
-      <c r="B34" s="58"/>
-      <c r="C34" s="58"/>
-      <c r="D34" s="58"/>
-      <c r="E34" s="58"/>
-      <c r="F34" s="58"/>
-      <c r="G34" s="58"/>
-      <c r="I34" s="58" t="s">
-        <v>85</v>
-      </c>
-      <c r="J34" s="58"/>
-      <c r="K34" s="58"/>
-      <c r="L34" s="58"/>
-      <c r="M34" s="58"/>
-      <c r="N34" s="58"/>
+      <c r="A34" s="73"/>
+      <c r="B34" s="70"/>
+      <c r="C34" s="70"/>
+      <c r="D34" s="70"/>
+      <c r="E34" s="70"/>
+      <c r="F34" s="70"/>
+      <c r="G34" s="74"/>
+      <c r="I34" s="23" t="s">
+        <v>84</v>
+      </c>
+      <c r="J34" s="23"/>
+      <c r="K34" s="23"/>
+      <c r="L34" s="23"/>
+      <c r="M34" s="23"/>
+      <c r="N34" s="23"/>
     </row>
     <row r="35" spans="1:14">
-      <c r="A35" s="58"/>
-      <c r="B35" s="58"/>
-      <c r="C35" s="58"/>
-      <c r="D35" s="58"/>
-      <c r="E35" s="58"/>
-      <c r="F35" s="58"/>
-      <c r="G35" s="58"/>
-      <c r="I35" s="58"/>
-      <c r="J35" s="58"/>
-      <c r="K35" s="58"/>
-      <c r="L35" s="58"/>
-      <c r="M35" s="58"/>
-      <c r="N35" s="58"/>
+      <c r="A35" s="73"/>
+      <c r="B35" s="70"/>
+      <c r="C35" s="70"/>
+      <c r="D35" s="70"/>
+      <c r="E35" s="70"/>
+      <c r="F35" s="70"/>
+      <c r="G35" s="74"/>
+      <c r="I35" s="23"/>
+      <c r="J35" s="23"/>
+      <c r="K35" s="23"/>
+      <c r="L35" s="23"/>
+      <c r="M35" s="23"/>
+      <c r="N35" s="23"/>
     </row>
     <row r="36" spans="1:14">
-      <c r="A36" s="58"/>
-      <c r="B36" s="58"/>
-      <c r="C36" s="58"/>
-      <c r="D36" s="58"/>
-      <c r="E36" s="58"/>
-      <c r="F36" s="58"/>
-      <c r="G36" s="58"/>
-      <c r="I36" s="54" t="s">
-        <v>95</v>
-      </c>
-      <c r="J36" s="54"/>
-      <c r="K36" s="54"/>
-      <c r="L36" s="54"/>
-      <c r="M36" s="54"/>
-      <c r="N36" s="54"/>
+      <c r="A36" s="73"/>
+      <c r="B36" s="70"/>
+      <c r="C36" s="70"/>
+      <c r="D36" s="70"/>
+      <c r="E36" s="70"/>
+      <c r="F36" s="70"/>
+      <c r="G36" s="74"/>
+      <c r="I36" s="19" t="s">
+        <v>94</v>
+      </c>
+      <c r="J36" s="19"/>
+      <c r="K36" s="19"/>
+      <c r="L36" s="19"/>
+      <c r="M36" s="19"/>
+      <c r="N36" s="19"/>
     </row>
     <row r="37" spans="1:14">
-      <c r="A37" s="58"/>
-      <c r="B37" s="58"/>
-      <c r="C37" s="58"/>
-      <c r="D37" s="58"/>
-      <c r="E37" s="58"/>
-      <c r="F37" s="58"/>
-      <c r="G37" s="58"/>
-      <c r="I37" s="53" t="s">
-        <v>97</v>
-      </c>
-      <c r="J37" s="53"/>
-      <c r="K37" s="53"/>
-      <c r="L37" s="53"/>
-      <c r="M37" s="53"/>
-      <c r="N37" s="53"/>
+      <c r="A37" s="73"/>
+      <c r="B37" s="70"/>
+      <c r="C37" s="70"/>
+      <c r="D37" s="70"/>
+      <c r="E37" s="70"/>
+      <c r="F37" s="70"/>
+      <c r="G37" s="74"/>
+      <c r="I37" s="18" t="s">
+        <v>96</v>
+      </c>
+      <c r="J37" s="18"/>
+      <c r="K37" s="18"/>
+      <c r="L37" s="18"/>
+      <c r="M37" s="18"/>
+      <c r="N37" s="18"/>
     </row>
     <row r="38" spans="1:14">
-      <c r="A38" s="58"/>
-      <c r="B38" s="58"/>
-      <c r="C38" s="58"/>
-      <c r="D38" s="58"/>
-      <c r="E38" s="58"/>
-      <c r="F38" s="58"/>
-      <c r="G38" s="58"/>
-      <c r="I38" s="53"/>
-      <c r="J38" s="53"/>
-      <c r="K38" s="53"/>
-      <c r="L38" s="53"/>
-      <c r="M38" s="53"/>
-      <c r="N38" s="53"/>
-    </row>
-    <row r="39" spans="1:14">
-      <c r="A39" s="13"/>
-      <c r="B39" s="13"/>
-      <c r="C39" s="13"/>
-      <c r="D39" s="13"/>
-      <c r="E39" s="13"/>
-      <c r="F39" s="13"/>
-      <c r="G39" s="13"/>
+      <c r="A38" s="73"/>
+      <c r="B38" s="70"/>
+      <c r="C38" s="70"/>
+      <c r="D38" s="70"/>
+      <c r="E38" s="70"/>
+      <c r="F38" s="70"/>
+      <c r="G38" s="74"/>
+      <c r="I38" s="18"/>
+      <c r="J38" s="18"/>
+      <c r="K38" s="18"/>
+      <c r="L38" s="18"/>
+      <c r="M38" s="18"/>
+      <c r="N38" s="18"/>
+    </row>
+    <row r="39" spans="1:14" ht="16" customHeight="1">
+      <c r="A39" s="75"/>
+      <c r="B39" s="76"/>
+      <c r="C39" s="76"/>
+      <c r="D39" s="76"/>
+      <c r="E39" s="76"/>
+      <c r="F39" s="76"/>
+      <c r="G39" s="77"/>
+      <c r="I39" s="66" t="s">
+        <v>100</v>
+      </c>
+      <c r="J39" s="67"/>
+      <c r="K39" s="67"/>
+      <c r="L39" s="67"/>
+      <c r="M39" s="67"/>
+      <c r="N39" s="68"/>
     </row>
     <row r="40" spans="1:14">
       <c r="A40" s="13"/>
@@ -2295,6 +2420,12 @@
       <c r="E40" s="13"/>
       <c r="F40" s="13"/>
       <c r="G40" s="13"/>
+      <c r="I40" s="65"/>
+      <c r="J40" s="65"/>
+      <c r="K40" s="65"/>
+      <c r="L40" s="65"/>
+      <c r="M40" s="65"/>
+      <c r="N40" s="65"/>
     </row>
     <row r="41" spans="1:14">
       <c r="A41" s="13"/>
@@ -2309,35 +2440,45 @@
       <c r="J44" s="14"/>
     </row>
   </sheetData>
-  <mergeCells count="80">
-    <mergeCell ref="M23:N23"/>
-    <mergeCell ref="M22:N22"/>
-    <mergeCell ref="I37:N38"/>
-    <mergeCell ref="I36:N36"/>
-    <mergeCell ref="A28:G28"/>
-    <mergeCell ref="A29:G29"/>
-    <mergeCell ref="A30:G30"/>
-    <mergeCell ref="I28:N28"/>
-    <mergeCell ref="A32:G38"/>
-    <mergeCell ref="I29:N30"/>
-    <mergeCell ref="I31:N33"/>
-    <mergeCell ref="I34:N35"/>
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="A2:D2"/>
-    <mergeCell ref="A1:G1"/>
-    <mergeCell ref="A4:A19"/>
-    <mergeCell ref="B4:B21"/>
-    <mergeCell ref="C4:C26"/>
-    <mergeCell ref="D4:D26"/>
-    <mergeCell ref="A20:A26"/>
-    <mergeCell ref="B22:B26"/>
-    <mergeCell ref="E24:E26"/>
-    <mergeCell ref="T24:U24"/>
-    <mergeCell ref="M24:N24"/>
-    <mergeCell ref="T25:U25"/>
-    <mergeCell ref="T26:U26"/>
-    <mergeCell ref="M25:N25"/>
-    <mergeCell ref="M26:N26"/>
+  <mergeCells count="81">
+    <mergeCell ref="I39:N39"/>
+    <mergeCell ref="A32:G39"/>
+    <mergeCell ref="M21:N21"/>
+    <mergeCell ref="M20:N20"/>
+    <mergeCell ref="I14:I19"/>
+    <mergeCell ref="K14:K16"/>
+    <mergeCell ref="N15:N16"/>
+    <mergeCell ref="K17:K19"/>
+    <mergeCell ref="N18:N19"/>
+    <mergeCell ref="J14:J19"/>
+    <mergeCell ref="I1:N1"/>
+    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="G2:G3"/>
+    <mergeCell ref="F8:F13"/>
+    <mergeCell ref="F14:F19"/>
+    <mergeCell ref="G8:G13"/>
+    <mergeCell ref="M4:N4"/>
+    <mergeCell ref="M6:N6"/>
+    <mergeCell ref="M7:N7"/>
+    <mergeCell ref="M5:N5"/>
+    <mergeCell ref="J8:J13"/>
+    <mergeCell ref="M2:N2"/>
+    <mergeCell ref="I2:L2"/>
+    <mergeCell ref="I8:I13"/>
+    <mergeCell ref="K8:K10"/>
+    <mergeCell ref="K11:K13"/>
+    <mergeCell ref="P1:U1"/>
+    <mergeCell ref="P2:S2"/>
+    <mergeCell ref="T2:U2"/>
+    <mergeCell ref="T4:U4"/>
+    <mergeCell ref="T5:U5"/>
+    <mergeCell ref="R8:R10"/>
+    <mergeCell ref="U9:U10"/>
+    <mergeCell ref="R11:R13"/>
+    <mergeCell ref="U12:U13"/>
+    <mergeCell ref="G14:G19"/>
+    <mergeCell ref="N9:N10"/>
+    <mergeCell ref="N12:N13"/>
     <mergeCell ref="T21:U21"/>
     <mergeCell ref="T20:U20"/>
     <mergeCell ref="T22:U22"/>
@@ -2354,42 +2495,33 @@
     <mergeCell ref="T7:U7"/>
     <mergeCell ref="P8:P13"/>
     <mergeCell ref="Q8:Q13"/>
-    <mergeCell ref="R8:R10"/>
-    <mergeCell ref="U9:U10"/>
-    <mergeCell ref="R11:R13"/>
-    <mergeCell ref="U12:U13"/>
-    <mergeCell ref="G14:G19"/>
-    <mergeCell ref="N9:N10"/>
-    <mergeCell ref="N12:N13"/>
-    <mergeCell ref="P1:U1"/>
-    <mergeCell ref="P2:S2"/>
-    <mergeCell ref="T2:U2"/>
-    <mergeCell ref="T4:U4"/>
-    <mergeCell ref="T5:U5"/>
-    <mergeCell ref="I1:N1"/>
-    <mergeCell ref="F2:F3"/>
-    <mergeCell ref="G2:G3"/>
-    <mergeCell ref="F8:F13"/>
-    <mergeCell ref="F14:F19"/>
-    <mergeCell ref="G8:G13"/>
-    <mergeCell ref="M4:N4"/>
-    <mergeCell ref="M6:N6"/>
-    <mergeCell ref="M7:N7"/>
-    <mergeCell ref="M5:N5"/>
-    <mergeCell ref="J8:J13"/>
-    <mergeCell ref="M2:N2"/>
-    <mergeCell ref="I2:L2"/>
-    <mergeCell ref="I8:I13"/>
-    <mergeCell ref="K8:K10"/>
-    <mergeCell ref="K11:K13"/>
-    <mergeCell ref="M21:N21"/>
-    <mergeCell ref="M20:N20"/>
-    <mergeCell ref="I14:I19"/>
-    <mergeCell ref="K14:K16"/>
-    <mergeCell ref="N15:N16"/>
-    <mergeCell ref="K17:K19"/>
-    <mergeCell ref="N18:N19"/>
-    <mergeCell ref="J14:J19"/>
+    <mergeCell ref="T24:U24"/>
+    <mergeCell ref="M24:N24"/>
+    <mergeCell ref="T25:U25"/>
+    <mergeCell ref="T26:U26"/>
+    <mergeCell ref="M25:N25"/>
+    <mergeCell ref="M26:N26"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="A4:A19"/>
+    <mergeCell ref="B4:B21"/>
+    <mergeCell ref="C4:C26"/>
+    <mergeCell ref="D4:D26"/>
+    <mergeCell ref="A20:A26"/>
+    <mergeCell ref="B22:B26"/>
+    <mergeCell ref="E24:E26"/>
+    <mergeCell ref="M23:N23"/>
+    <mergeCell ref="M22:N22"/>
+    <mergeCell ref="I37:N38"/>
+    <mergeCell ref="I36:N36"/>
+    <mergeCell ref="A28:G28"/>
+    <mergeCell ref="A29:G29"/>
+    <mergeCell ref="A30:G30"/>
+    <mergeCell ref="I28:N28"/>
+    <mergeCell ref="I29:N30"/>
+    <mergeCell ref="I31:N33"/>
+    <mergeCell ref="I34:N35"/>
   </mergeCells>
   <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="59" fitToHeight="0" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
v7.7: LCD dashboard, Neopixels, SUMD support
</commit_message>
<xml_diff>
--- a/adjustmentsRemote.xlsx
+++ b/adjustmentsRemote.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10808"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/martinsommer/Documents/Programmieren/GitHub/RC/Rc_Engine_Sound_ESP32/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3EC101E-8D65-3748-B7E4-9049196E76CB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{168B8D9E-B71E-3A45-8A5C-758DDBE9C2AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2140" yWindow="1380" windowWidth="46720" windowHeight="24940" xr2:uid="{7FD8C6E5-3068-1C47-BC39-03FF60370E8F}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="100">
   <si>
     <t>up</t>
   </si>
@@ -256,9 +256,6 @@
   </si>
   <si>
     <t>IBUS</t>
-  </si>
-  <si>
-    <t>Yes, SBUS</t>
   </si>
   <si>
     <t>Sound controller channel</t>
@@ -731,6 +728,108 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -740,6 +839,66 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -756,168 +915,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1289,7 +1286,7 @@
   <dimension ref="A1:U44"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="J44" sqref="J44"/>
+      <selection activeCell="E4" sqref="E4:E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1315,68 +1312,68 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="63" t="s">
         <v>34</v>
       </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
-      <c r="F1" s="27"/>
-      <c r="G1" s="28"/>
-      <c r="I1" s="58" t="s">
+      <c r="B1" s="63"/>
+      <c r="C1" s="63"/>
+      <c r="D1" s="63"/>
+      <c r="E1" s="63"/>
+      <c r="F1" s="63"/>
+      <c r="G1" s="64"/>
+      <c r="I1" s="36" t="s">
         <v>33</v>
       </c>
-      <c r="J1" s="58"/>
-      <c r="K1" s="58"/>
-      <c r="L1" s="58"/>
-      <c r="M1" s="58"/>
-      <c r="N1" s="58"/>
-      <c r="P1" s="56" t="s">
+      <c r="J1" s="36"/>
+      <c r="K1" s="36"/>
+      <c r="L1" s="36"/>
+      <c r="M1" s="36"/>
+      <c r="N1" s="36"/>
+      <c r="P1" s="48" t="s">
         <v>68</v>
       </c>
-      <c r="Q1" s="56"/>
-      <c r="R1" s="56"/>
-      <c r="S1" s="56"/>
-      <c r="T1" s="56"/>
-      <c r="U1" s="56"/>
+      <c r="Q1" s="48"/>
+      <c r="R1" s="48"/>
+      <c r="S1" s="48"/>
+      <c r="T1" s="48"/>
+      <c r="U1" s="48"/>
     </row>
     <row r="2" spans="1:21">
-      <c r="A2" s="26" t="s">
-        <v>86</v>
-      </c>
-      <c r="B2" s="26"/>
-      <c r="C2" s="26"/>
-      <c r="D2" s="26"/>
-      <c r="E2" s="24" t="s">
+      <c r="A2" s="62" t="s">
+        <v>85</v>
+      </c>
+      <c r="B2" s="62"/>
+      <c r="C2" s="62"/>
+      <c r="D2" s="62"/>
+      <c r="E2" s="39" t="s">
         <v>71</v>
       </c>
-      <c r="F2" s="59" t="s">
-        <v>77</v>
-      </c>
-      <c r="G2" s="24" t="s">
+      <c r="F2" s="37" t="s">
+        <v>76</v>
+      </c>
+      <c r="G2" s="39" t="s">
         <v>17</v>
       </c>
-      <c r="I2" s="57" t="s">
+      <c r="I2" s="47" t="s">
         <v>28</v>
       </c>
-      <c r="J2" s="57"/>
-      <c r="K2" s="57"/>
-      <c r="L2" s="57"/>
-      <c r="M2" s="57" t="s">
+      <c r="J2" s="47"/>
+      <c r="K2" s="47"/>
+      <c r="L2" s="47"/>
+      <c r="M2" s="47" t="s">
         <v>27</v>
       </c>
-      <c r="N2" s="57"/>
-      <c r="P2" s="57" t="s">
+      <c r="N2" s="47"/>
+      <c r="P2" s="47" t="s">
         <v>28</v>
       </c>
-      <c r="Q2" s="57"/>
-      <c r="R2" s="57"/>
-      <c r="S2" s="57"/>
-      <c r="T2" s="57" t="s">
+      <c r="Q2" s="47"/>
+      <c r="R2" s="47"/>
+      <c r="S2" s="47"/>
+      <c r="T2" s="47" t="s">
         <v>27</v>
       </c>
-      <c r="U2" s="57"/>
+      <c r="U2" s="47"/>
     </row>
     <row r="3" spans="1:21" ht="32" customHeight="1">
       <c r="A3" s="2" t="s">
@@ -1391,11 +1388,11 @@
       <c r="D3" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="E3" s="25"/>
-      <c r="F3" s="60"/>
-      <c r="G3" s="25"/>
+      <c r="E3" s="40"/>
+      <c r="F3" s="38"/>
+      <c r="G3" s="40"/>
       <c r="I3" s="10" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="J3" s="2" t="s">
         <v>17</v>
@@ -1413,7 +1410,7 @@
         <v>26</v>
       </c>
       <c r="P3" s="10" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="Q3" s="2" t="s">
         <v>17</v>
@@ -1432,19 +1429,19 @@
       </c>
     </row>
     <row r="4" spans="1:21">
-      <c r="A4" s="29" t="s">
-        <v>79</v>
-      </c>
-      <c r="B4" s="29" t="s">
-        <v>87</v>
-      </c>
-      <c r="C4" s="29" t="s">
-        <v>76</v>
-      </c>
-      <c r="D4" s="29" t="s">
-        <v>87</v>
-      </c>
-      <c r="E4" s="39" t="s">
+      <c r="A4" s="65" t="s">
+        <v>78</v>
+      </c>
+      <c r="B4" s="65" t="s">
+        <v>86</v>
+      </c>
+      <c r="C4" s="65" t="s">
+        <v>86</v>
+      </c>
+      <c r="D4" s="65" t="s">
+        <v>86</v>
+      </c>
+      <c r="E4" s="52" t="s">
         <v>56</v>
       </c>
       <c r="F4" s="11">
@@ -1461,10 +1458,10 @@
       </c>
       <c r="K4" s="1"/>
       <c r="L4" s="1"/>
-      <c r="M4" s="38" t="s">
+      <c r="M4" s="28" t="s">
         <v>21</v>
       </c>
-      <c r="N4" s="38"/>
+      <c r="N4" s="28"/>
       <c r="P4" s="4">
         <v>1</v>
       </c>
@@ -1473,17 +1470,17 @@
       </c>
       <c r="R4" s="1"/>
       <c r="S4" s="1"/>
-      <c r="T4" s="38" t="s">
+      <c r="T4" s="28" t="s">
         <v>21</v>
       </c>
-      <c r="U4" s="38"/>
+      <c r="U4" s="28"/>
     </row>
     <row r="5" spans="1:21">
-      <c r="A5" s="29"/>
-      <c r="B5" s="29"/>
-      <c r="C5" s="29"/>
-      <c r="D5" s="29"/>
-      <c r="E5" s="39"/>
+      <c r="A5" s="65"/>
+      <c r="B5" s="65"/>
+      <c r="C5" s="65"/>
+      <c r="D5" s="65"/>
+      <c r="E5" s="52"/>
       <c r="F5" s="11">
         <v>2</v>
       </c>
@@ -1498,10 +1495,10 @@
       </c>
       <c r="K5" s="1"/>
       <c r="L5" s="1"/>
-      <c r="M5" s="38" t="s">
+      <c r="M5" s="28" t="s">
         <v>39</v>
       </c>
-      <c r="N5" s="38"/>
+      <c r="N5" s="28"/>
       <c r="P5" s="4">
         <v>2</v>
       </c>
@@ -1510,17 +1507,17 @@
       </c>
       <c r="R5" s="1"/>
       <c r="S5" s="1"/>
-      <c r="T5" s="38" t="s">
+      <c r="T5" s="28" t="s">
         <v>39</v>
       </c>
-      <c r="U5" s="38"/>
+      <c r="U5" s="28"/>
     </row>
     <row r="6" spans="1:21">
-      <c r="A6" s="29"/>
-      <c r="B6" s="29"/>
-      <c r="C6" s="29"/>
-      <c r="D6" s="29"/>
-      <c r="E6" s="39"/>
+      <c r="A6" s="65"/>
+      <c r="B6" s="65"/>
+      <c r="C6" s="65"/>
+      <c r="D6" s="65"/>
+      <c r="E6" s="52"/>
       <c r="F6" s="11">
         <v>3</v>
       </c>
@@ -1535,10 +1532,10 @@
       </c>
       <c r="K6" s="1"/>
       <c r="L6" s="1"/>
-      <c r="M6" s="38" t="s">
+      <c r="M6" s="28" t="s">
         <v>23</v>
       </c>
-      <c r="N6" s="38"/>
+      <c r="N6" s="28"/>
       <c r="P6" s="4">
         <v>3</v>
       </c>
@@ -1547,17 +1544,17 @@
       </c>
       <c r="R6" s="1"/>
       <c r="S6" s="1"/>
-      <c r="T6" s="38" t="s">
+      <c r="T6" s="28" t="s">
         <v>23</v>
       </c>
-      <c r="U6" s="38"/>
+      <c r="U6" s="28"/>
     </row>
     <row r="7" spans="1:21">
-      <c r="A7" s="29"/>
-      <c r="B7" s="29"/>
-      <c r="C7" s="29"/>
-      <c r="D7" s="29"/>
-      <c r="E7" s="39"/>
+      <c r="A7" s="65"/>
+      <c r="B7" s="65"/>
+      <c r="C7" s="65"/>
+      <c r="D7" s="65"/>
+      <c r="E7" s="52"/>
       <c r="F7" s="11">
         <v>4</v>
       </c>
@@ -1572,10 +1569,10 @@
       </c>
       <c r="K7" s="1"/>
       <c r="L7" s="1"/>
-      <c r="M7" s="38" t="s">
+      <c r="M7" s="28" t="s">
         <v>41</v>
       </c>
-      <c r="N7" s="38"/>
+      <c r="N7" s="28"/>
       <c r="P7" s="4">
         <v>5</v>
       </c>
@@ -1584,30 +1581,30 @@
       </c>
       <c r="R7" s="1"/>
       <c r="S7" s="1"/>
-      <c r="T7" s="38" t="s">
+      <c r="T7" s="28" t="s">
         <v>41</v>
       </c>
-      <c r="U7" s="38"/>
+      <c r="U7" s="28"/>
     </row>
     <row r="8" spans="1:21">
-      <c r="A8" s="29"/>
-      <c r="B8" s="29"/>
-      <c r="C8" s="29"/>
-      <c r="D8" s="29"/>
-      <c r="E8" s="39"/>
-      <c r="F8" s="61">
+      <c r="A8" s="65"/>
+      <c r="B8" s="65"/>
+      <c r="C8" s="65"/>
+      <c r="D8" s="65"/>
+      <c r="E8" s="52"/>
+      <c r="F8" s="41">
         <v>5</v>
       </c>
-      <c r="G8" s="53" t="s">
+      <c r="G8" s="44" t="s">
         <v>36</v>
       </c>
-      <c r="I8" s="47">
+      <c r="I8" s="30">
         <v>2</v>
       </c>
-      <c r="J8" s="48" t="s">
+      <c r="J8" s="33" t="s">
         <v>19</v>
       </c>
-      <c r="K8" s="51" t="s">
+      <c r="K8" s="31" t="s">
         <v>0</v>
       </c>
       <c r="L8" s="1" t="s">
@@ -1619,13 +1616,13 @@
       <c r="N8" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="P8" s="47">
+      <c r="P8" s="30">
         <v>4</v>
       </c>
-      <c r="Q8" s="48" t="s">
-        <v>83</v>
-      </c>
-      <c r="R8" s="51" t="s">
+      <c r="Q8" s="33" t="s">
+        <v>82</v>
+      </c>
+      <c r="R8" s="31" t="s">
         <v>12</v>
       </c>
       <c r="S8" s="1" t="s">
@@ -1639,169 +1636,169 @@
       </c>
     </row>
     <row r="9" spans="1:21">
-      <c r="A9" s="29"/>
-      <c r="B9" s="29"/>
-      <c r="C9" s="29"/>
-      <c r="D9" s="29"/>
-      <c r="E9" s="39"/>
-      <c r="F9" s="62"/>
-      <c r="G9" s="54"/>
-      <c r="I9" s="47"/>
-      <c r="J9" s="49"/>
-      <c r="K9" s="51"/>
+      <c r="A9" s="65"/>
+      <c r="B9" s="65"/>
+      <c r="C9" s="65"/>
+      <c r="D9" s="65"/>
+      <c r="E9" s="52"/>
+      <c r="F9" s="42"/>
+      <c r="G9" s="45"/>
+      <c r="I9" s="30"/>
+      <c r="J9" s="34"/>
+      <c r="K9" s="31"/>
       <c r="L9" s="1" t="s">
         <v>6</v>
       </c>
       <c r="M9" s="1"/>
-      <c r="N9" s="52"/>
-      <c r="P9" s="47"/>
-      <c r="Q9" s="49"/>
-      <c r="R9" s="51"/>
+      <c r="N9" s="32"/>
+      <c r="P9" s="30"/>
+      <c r="Q9" s="34"/>
+      <c r="R9" s="31"/>
       <c r="S9" s="1" t="s">
         <v>6</v>
       </c>
       <c r="T9" s="1"/>
-      <c r="U9" s="52"/>
+      <c r="U9" s="32"/>
     </row>
     <row r="10" spans="1:21">
-      <c r="A10" s="29"/>
-      <c r="B10" s="29"/>
-      <c r="C10" s="29"/>
-      <c r="D10" s="29"/>
-      <c r="E10" s="39"/>
-      <c r="F10" s="62"/>
-      <c r="G10" s="54"/>
-      <c r="I10" s="47"/>
-      <c r="J10" s="49"/>
-      <c r="K10" s="51"/>
+      <c r="A10" s="65"/>
+      <c r="B10" s="65"/>
+      <c r="C10" s="65"/>
+      <c r="D10" s="65"/>
+      <c r="E10" s="52"/>
+      <c r="F10" s="42"/>
+      <c r="G10" s="45"/>
+      <c r="I10" s="30"/>
+      <c r="J10" s="34"/>
+      <c r="K10" s="31"/>
       <c r="L10" s="1" t="s">
         <v>7</v>
       </c>
       <c r="M10" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="N10" s="52"/>
-      <c r="P10" s="47"/>
-      <c r="Q10" s="49"/>
-      <c r="R10" s="51"/>
+      <c r="N10" s="32"/>
+      <c r="P10" s="30"/>
+      <c r="Q10" s="34"/>
+      <c r="R10" s="31"/>
       <c r="S10" s="1" t="s">
         <v>7</v>
       </c>
       <c r="T10" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="U10" s="52"/>
+      <c r="U10" s="32"/>
     </row>
     <row r="11" spans="1:21">
-      <c r="A11" s="29"/>
-      <c r="B11" s="29"/>
-      <c r="C11" s="29"/>
-      <c r="D11" s="29"/>
-      <c r="E11" s="39"/>
-      <c r="F11" s="62"/>
-      <c r="G11" s="54"/>
-      <c r="I11" s="47"/>
-      <c r="J11" s="49"/>
-      <c r="K11" s="51" t="s">
+      <c r="A11" s="65"/>
+      <c r="B11" s="65"/>
+      <c r="C11" s="65"/>
+      <c r="D11" s="65"/>
+      <c r="E11" s="52"/>
+      <c r="F11" s="42"/>
+      <c r="G11" s="45"/>
+      <c r="I11" s="30"/>
+      <c r="J11" s="34"/>
+      <c r="K11" s="31" t="s">
         <v>1</v>
       </c>
       <c r="L11" s="1" t="s">
         <v>5</v>
       </c>
       <c r="M11" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="N11" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="P11" s="47"/>
-      <c r="Q11" s="49"/>
-      <c r="R11" s="51" t="s">
+      <c r="P11" s="30"/>
+      <c r="Q11" s="34"/>
+      <c r="R11" s="31" t="s">
         <v>13</v>
       </c>
       <c r="S11" s="1" t="s">
         <v>5</v>
       </c>
       <c r="T11" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="U11" s="8" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="12" spans="1:21">
-      <c r="A12" s="29"/>
-      <c r="B12" s="29"/>
-      <c r="C12" s="29"/>
-      <c r="D12" s="29"/>
-      <c r="E12" s="39"/>
-      <c r="F12" s="62"/>
-      <c r="G12" s="54"/>
-      <c r="I12" s="47"/>
-      <c r="J12" s="49"/>
-      <c r="K12" s="51"/>
+      <c r="A12" s="65"/>
+      <c r="B12" s="65"/>
+      <c r="C12" s="65"/>
+      <c r="D12" s="65"/>
+      <c r="E12" s="52"/>
+      <c r="F12" s="42"/>
+      <c r="G12" s="45"/>
+      <c r="I12" s="30"/>
+      <c r="J12" s="34"/>
+      <c r="K12" s="31"/>
       <c r="L12" s="1" t="s">
         <v>6</v>
       </c>
       <c r="M12" s="1"/>
-      <c r="N12" s="52"/>
-      <c r="P12" s="47"/>
-      <c r="Q12" s="49"/>
-      <c r="R12" s="51"/>
+      <c r="N12" s="32"/>
+      <c r="P12" s="30"/>
+      <c r="Q12" s="34"/>
+      <c r="R12" s="31"/>
       <c r="S12" s="1" t="s">
         <v>6</v>
       </c>
       <c r="T12" s="1"/>
-      <c r="U12" s="52"/>
+      <c r="U12" s="32"/>
     </row>
     <row r="13" spans="1:21">
-      <c r="A13" s="29"/>
-      <c r="B13" s="29"/>
-      <c r="C13" s="29"/>
-      <c r="D13" s="29"/>
-      <c r="E13" s="39"/>
-      <c r="F13" s="63"/>
-      <c r="G13" s="55"/>
-      <c r="I13" s="47"/>
-      <c r="J13" s="50"/>
-      <c r="K13" s="51"/>
+      <c r="A13" s="65"/>
+      <c r="B13" s="65"/>
+      <c r="C13" s="65"/>
+      <c r="D13" s="65"/>
+      <c r="E13" s="52"/>
+      <c r="F13" s="43"/>
+      <c r="G13" s="46"/>
+      <c r="I13" s="30"/>
+      <c r="J13" s="35"/>
+      <c r="K13" s="31"/>
       <c r="L13" s="1" t="s">
         <v>7</v>
       </c>
       <c r="M13" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="N13" s="52"/>
-      <c r="P13" s="47"/>
-      <c r="Q13" s="50"/>
-      <c r="R13" s="51"/>
+      <c r="N13" s="32"/>
+      <c r="P13" s="30"/>
+      <c r="Q13" s="35"/>
+      <c r="R13" s="31"/>
       <c r="S13" s="1" t="s">
         <v>7</v>
       </c>
       <c r="T13" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="U13" s="52"/>
+      <c r="U13" s="32"/>
     </row>
     <row r="14" spans="1:21">
-      <c r="A14" s="29"/>
-      <c r="B14" s="29"/>
-      <c r="C14" s="29"/>
-      <c r="D14" s="29"/>
-      <c r="E14" s="39"/>
-      <c r="F14" s="61">
+      <c r="A14" s="65"/>
+      <c r="B14" s="65"/>
+      <c r="C14" s="65"/>
+      <c r="D14" s="65"/>
+      <c r="E14" s="52"/>
+      <c r="F14" s="41">
         <v>6</v>
       </c>
-      <c r="G14" s="53" t="s">
+      <c r="G14" s="44" t="s">
         <v>37</v>
       </c>
-      <c r="I14" s="47">
+      <c r="I14" s="30">
         <v>4</v>
       </c>
-      <c r="J14" s="48" t="s">
+      <c r="J14" s="33" t="s">
         <v>20</v>
       </c>
-      <c r="K14" s="51" t="s">
+      <c r="K14" s="31" t="s">
         <v>12</v>
       </c>
       <c r="L14" s="1" t="s">
@@ -1811,11 +1808,11 @@
       <c r="N14" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P14" s="42">
+      <c r="P14" s="55">
         <v>16</v>
       </c>
-      <c r="Q14" s="43"/>
-      <c r="R14" s="42"/>
+      <c r="Q14" s="56"/>
+      <c r="R14" s="55"/>
       <c r="S14" s="6" t="s">
         <v>5</v>
       </c>
@@ -1823,68 +1820,68 @@
       <c r="U14" s="6"/>
     </row>
     <row r="15" spans="1:21">
-      <c r="A15" s="29"/>
-      <c r="B15" s="29"/>
-      <c r="C15" s="29"/>
-      <c r="D15" s="29"/>
-      <c r="E15" s="39"/>
-      <c r="F15" s="62"/>
-      <c r="G15" s="54"/>
-      <c r="I15" s="47"/>
-      <c r="J15" s="49"/>
-      <c r="K15" s="51"/>
+      <c r="A15" s="65"/>
+      <c r="B15" s="65"/>
+      <c r="C15" s="65"/>
+      <c r="D15" s="65"/>
+      <c r="E15" s="52"/>
+      <c r="F15" s="42"/>
+      <c r="G15" s="45"/>
+      <c r="I15" s="30"/>
+      <c r="J15" s="34"/>
+      <c r="K15" s="31"/>
       <c r="L15" s="1" t="s">
         <v>6</v>
       </c>
       <c r="M15" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="N15" s="52"/>
-      <c r="P15" s="42"/>
-      <c r="Q15" s="44"/>
-      <c r="R15" s="42"/>
+      <c r="N15" s="32"/>
+      <c r="P15" s="55"/>
+      <c r="Q15" s="57"/>
+      <c r="R15" s="55"/>
       <c r="S15" s="6" t="s">
         <v>6</v>
       </c>
       <c r="T15" s="6"/>
-      <c r="U15" s="46"/>
+      <c r="U15" s="59"/>
     </row>
     <row r="16" spans="1:21">
-      <c r="A16" s="29"/>
-      <c r="B16" s="29"/>
-      <c r="C16" s="29"/>
-      <c r="D16" s="29"/>
-      <c r="E16" s="39"/>
-      <c r="F16" s="62"/>
-      <c r="G16" s="54"/>
-      <c r="I16" s="47"/>
-      <c r="J16" s="49"/>
-      <c r="K16" s="51"/>
+      <c r="A16" s="65"/>
+      <c r="B16" s="65"/>
+      <c r="C16" s="65"/>
+      <c r="D16" s="65"/>
+      <c r="E16" s="52"/>
+      <c r="F16" s="42"/>
+      <c r="G16" s="45"/>
+      <c r="I16" s="30"/>
+      <c r="J16" s="34"/>
+      <c r="K16" s="31"/>
       <c r="L16" s="1" t="s">
         <v>7</v>
       </c>
       <c r="M16" s="1"/>
-      <c r="N16" s="52"/>
-      <c r="P16" s="42"/>
-      <c r="Q16" s="44"/>
-      <c r="R16" s="42"/>
+      <c r="N16" s="32"/>
+      <c r="P16" s="55"/>
+      <c r="Q16" s="57"/>
+      <c r="R16" s="55"/>
       <c r="S16" s="6" t="s">
         <v>7</v>
       </c>
       <c r="T16" s="6"/>
-      <c r="U16" s="46"/>
+      <c r="U16" s="59"/>
     </row>
     <row r="17" spans="1:21">
-      <c r="A17" s="29"/>
-      <c r="B17" s="29"/>
-      <c r="C17" s="29"/>
-      <c r="D17" s="29"/>
-      <c r="E17" s="39"/>
-      <c r="F17" s="62"/>
-      <c r="G17" s="54"/>
-      <c r="I17" s="47"/>
-      <c r="J17" s="49"/>
-      <c r="K17" s="51" t="s">
+      <c r="A17" s="65"/>
+      <c r="B17" s="65"/>
+      <c r="C17" s="65"/>
+      <c r="D17" s="65"/>
+      <c r="E17" s="52"/>
+      <c r="F17" s="42"/>
+      <c r="G17" s="45"/>
+      <c r="I17" s="30"/>
+      <c r="J17" s="34"/>
+      <c r="K17" s="31" t="s">
         <v>13</v>
       </c>
       <c r="L17" s="1" t="s">
@@ -1892,11 +1889,11 @@
       </c>
       <c r="M17" s="1"/>
       <c r="N17" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="P17" s="42"/>
-      <c r="Q17" s="44"/>
-      <c r="R17" s="42"/>
+        <v>97</v>
+      </c>
+      <c r="P17" s="55"/>
+      <c r="Q17" s="57"/>
+      <c r="R17" s="55"/>
       <c r="S17" s="6" t="s">
         <v>5</v>
       </c>
@@ -1904,70 +1901,70 @@
       <c r="U17" s="6"/>
     </row>
     <row r="18" spans="1:21">
-      <c r="A18" s="29"/>
-      <c r="B18" s="29"/>
-      <c r="C18" s="29"/>
-      <c r="D18" s="29"/>
-      <c r="E18" s="39"/>
-      <c r="F18" s="62"/>
-      <c r="G18" s="54"/>
-      <c r="I18" s="47"/>
-      <c r="J18" s="49"/>
-      <c r="K18" s="51"/>
+      <c r="A18" s="65"/>
+      <c r="B18" s="65"/>
+      <c r="C18" s="65"/>
+      <c r="D18" s="65"/>
+      <c r="E18" s="52"/>
+      <c r="F18" s="42"/>
+      <c r="G18" s="45"/>
+      <c r="I18" s="30"/>
+      <c r="J18" s="34"/>
+      <c r="K18" s="31"/>
       <c r="L18" s="1" t="s">
         <v>6</v>
       </c>
       <c r="M18" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="N18" s="52"/>
-      <c r="P18" s="42"/>
-      <c r="Q18" s="44"/>
-      <c r="R18" s="42"/>
+      <c r="N18" s="32"/>
+      <c r="P18" s="55"/>
+      <c r="Q18" s="57"/>
+      <c r="R18" s="55"/>
       <c r="S18" s="6" t="s">
         <v>6</v>
       </c>
       <c r="T18" s="6"/>
-      <c r="U18" s="46"/>
+      <c r="U18" s="59"/>
     </row>
     <row r="19" spans="1:21">
-      <c r="A19" s="29"/>
-      <c r="B19" s="29"/>
-      <c r="C19" s="29"/>
-      <c r="D19" s="29"/>
-      <c r="E19" s="39"/>
-      <c r="F19" s="63"/>
-      <c r="G19" s="55"/>
-      <c r="I19" s="47"/>
-      <c r="J19" s="50"/>
-      <c r="K19" s="51"/>
+      <c r="A19" s="65"/>
+      <c r="B19" s="65"/>
+      <c r="C19" s="65"/>
+      <c r="D19" s="65"/>
+      <c r="E19" s="52"/>
+      <c r="F19" s="43"/>
+      <c r="G19" s="46"/>
+      <c r="I19" s="30"/>
+      <c r="J19" s="35"/>
+      <c r="K19" s="31"/>
       <c r="L19" s="1" t="s">
         <v>7</v>
       </c>
       <c r="M19" s="1"/>
-      <c r="N19" s="52"/>
-      <c r="P19" s="42"/>
-      <c r="Q19" s="45"/>
-      <c r="R19" s="42"/>
+      <c r="N19" s="32"/>
+      <c r="P19" s="55"/>
+      <c r="Q19" s="58"/>
+      <c r="R19" s="55"/>
       <c r="S19" s="6" t="s">
         <v>7</v>
       </c>
       <c r="T19" s="6"/>
-      <c r="U19" s="46"/>
+      <c r="U19" s="59"/>
     </row>
     <row r="20" spans="1:21">
-      <c r="A20" s="30" t="s">
-        <v>88</v>
-      </c>
-      <c r="B20" s="29"/>
-      <c r="C20" s="29"/>
-      <c r="D20" s="29"/>
-      <c r="E20" s="39"/>
+      <c r="A20" s="66" t="s">
+        <v>87</v>
+      </c>
+      <c r="B20" s="65"/>
+      <c r="C20" s="65"/>
+      <c r="D20" s="65"/>
+      <c r="E20" s="52"/>
       <c r="F20" s="11">
         <v>7</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="I20" s="4">
         <v>8</v>
@@ -1977,27 +1974,27 @@
       </c>
       <c r="K20" s="1"/>
       <c r="L20" s="1"/>
-      <c r="M20" s="64" t="s">
-        <v>90</v>
-      </c>
-      <c r="N20" s="64"/>
+      <c r="M20" s="29" t="s">
+        <v>89</v>
+      </c>
+      <c r="N20" s="29"/>
       <c r="P20" s="7">
         <v>16</v>
       </c>
       <c r="Q20" s="6"/>
       <c r="R20" s="6"/>
       <c r="S20" s="6"/>
-      <c r="T20" s="15" t="s">
+      <c r="T20" s="49" t="s">
         <v>45</v>
       </c>
-      <c r="U20" s="15"/>
+      <c r="U20" s="49"/>
     </row>
     <row r="21" spans="1:21" ht="16" customHeight="1">
-      <c r="A21" s="31"/>
-      <c r="B21" s="29"/>
-      <c r="C21" s="29"/>
-      <c r="D21" s="29"/>
-      <c r="E21" s="40" t="s">
+      <c r="A21" s="67"/>
+      <c r="B21" s="65"/>
+      <c r="C21" s="65"/>
+      <c r="D21" s="65"/>
+      <c r="E21" s="53" t="s">
         <v>59</v>
       </c>
       <c r="F21" s="11">
@@ -2014,10 +2011,10 @@
       </c>
       <c r="K21" s="1"/>
       <c r="L21" s="1"/>
-      <c r="M21" s="38" t="s">
-        <v>95</v>
-      </c>
-      <c r="N21" s="38"/>
+      <c r="M21" s="28" t="s">
+        <v>94</v>
+      </c>
+      <c r="N21" s="28"/>
       <c r="P21" s="4">
         <v>6</v>
       </c>
@@ -2026,19 +2023,19 @@
       </c>
       <c r="R21" s="1"/>
       <c r="S21" s="1"/>
-      <c r="T21" s="38" t="s">
-        <v>95</v>
-      </c>
-      <c r="U21" s="38"/>
+      <c r="T21" s="28" t="s">
+        <v>94</v>
+      </c>
+      <c r="U21" s="28"/>
     </row>
     <row r="22" spans="1:21">
-      <c r="A22" s="31"/>
-      <c r="B22" s="30" t="s">
-        <v>88</v>
-      </c>
-      <c r="C22" s="29"/>
-      <c r="D22" s="29"/>
-      <c r="E22" s="41"/>
+      <c r="A22" s="67"/>
+      <c r="B22" s="66" t="s">
+        <v>87</v>
+      </c>
+      <c r="C22" s="65"/>
+      <c r="D22" s="65"/>
+      <c r="E22" s="54"/>
       <c r="F22" s="11">
         <v>9</v>
       </c>
@@ -2053,10 +2050,10 @@
       </c>
       <c r="K22" s="1"/>
       <c r="L22" s="1"/>
-      <c r="M22" s="16" t="s">
-        <v>91</v>
-      </c>
-      <c r="N22" s="17"/>
+      <c r="M22" s="50" t="s">
+        <v>90</v>
+      </c>
+      <c r="N22" s="51"/>
       <c r="P22" s="4">
         <v>7</v>
       </c>
@@ -2065,16 +2062,16 @@
       </c>
       <c r="R22" s="1"/>
       <c r="S22" s="1"/>
-      <c r="T22" s="16" t="s">
-        <v>91</v>
-      </c>
-      <c r="U22" s="17"/>
+      <c r="T22" s="50" t="s">
+        <v>90</v>
+      </c>
+      <c r="U22" s="51"/>
     </row>
     <row r="23" spans="1:21" ht="17">
-      <c r="A23" s="31"/>
-      <c r="B23" s="31"/>
-      <c r="C23" s="29"/>
-      <c r="D23" s="29"/>
+      <c r="A23" s="67"/>
+      <c r="B23" s="67"/>
+      <c r="C23" s="65"/>
+      <c r="D23" s="65"/>
       <c r="E23" s="12" t="s">
         <v>7</v>
       </c>
@@ -2090,10 +2087,10 @@
       <c r="J23" s="6"/>
       <c r="K23" s="6"/>
       <c r="L23" s="6"/>
-      <c r="M23" s="15" t="s">
+      <c r="M23" s="49" t="s">
         <v>69</v>
       </c>
-      <c r="N23" s="15"/>
+      <c r="N23" s="49"/>
       <c r="P23" s="4">
         <v>8</v>
       </c>
@@ -2102,17 +2099,17 @@
       </c>
       <c r="R23" s="1"/>
       <c r="S23" s="1"/>
-      <c r="T23" s="16" t="s">
+      <c r="T23" s="50" t="s">
         <v>10</v>
       </c>
-      <c r="U23" s="17"/>
+      <c r="U23" s="51"/>
     </row>
     <row r="24" spans="1:21">
-      <c r="A24" s="31"/>
-      <c r="B24" s="31"/>
-      <c r="C24" s="29"/>
-      <c r="D24" s="29"/>
-      <c r="E24" s="33" t="s">
+      <c r="A24" s="67"/>
+      <c r="B24" s="67"/>
+      <c r="C24" s="65"/>
+      <c r="D24" s="65"/>
+      <c r="E24" s="69" t="s">
         <v>57</v>
       </c>
       <c r="F24" s="11">
@@ -2127,10 +2124,10 @@
       <c r="J24" s="6"/>
       <c r="K24" s="6"/>
       <c r="L24" s="6"/>
-      <c r="M24" s="15" t="s">
+      <c r="M24" s="49" t="s">
         <v>45</v>
       </c>
-      <c r="N24" s="15"/>
+      <c r="N24" s="49"/>
       <c r="P24" s="4">
         <v>9</v>
       </c>
@@ -2139,17 +2136,17 @@
       </c>
       <c r="R24" s="1"/>
       <c r="S24" s="1"/>
-      <c r="T24" s="16" t="s">
+      <c r="T24" s="50" t="s">
         <v>60</v>
       </c>
-      <c r="U24" s="17"/>
+      <c r="U24" s="51"/>
     </row>
     <row r="25" spans="1:21">
-      <c r="A25" s="31"/>
-      <c r="B25" s="31"/>
-      <c r="C25" s="29"/>
-      <c r="D25" s="29"/>
-      <c r="E25" s="34"/>
+      <c r="A25" s="67"/>
+      <c r="B25" s="67"/>
+      <c r="C25" s="65"/>
+      <c r="D25" s="65"/>
+      <c r="E25" s="70"/>
       <c r="F25" s="11">
         <v>12</v>
       </c>
@@ -2162,10 +2159,10 @@
       <c r="J25" s="6"/>
       <c r="K25" s="6"/>
       <c r="L25" s="6"/>
-      <c r="M25" s="15" t="s">
+      <c r="M25" s="49" t="s">
         <v>45</v>
       </c>
-      <c r="N25" s="15"/>
+      <c r="N25" s="49"/>
       <c r="P25" s="4">
         <v>10</v>
       </c>
@@ -2174,17 +2171,17 @@
       </c>
       <c r="R25" s="1"/>
       <c r="S25" s="1"/>
-      <c r="T25" s="36" t="s">
+      <c r="T25" s="60" t="s">
         <v>62</v>
       </c>
-      <c r="U25" s="37"/>
+      <c r="U25" s="61"/>
     </row>
     <row r="26" spans="1:21">
-      <c r="A26" s="32"/>
-      <c r="B26" s="31"/>
-      <c r="C26" s="29"/>
-      <c r="D26" s="29"/>
-      <c r="E26" s="35"/>
+      <c r="A26" s="68"/>
+      <c r="B26" s="67"/>
+      <c r="C26" s="65"/>
+      <c r="D26" s="65"/>
+      <c r="E26" s="71"/>
       <c r="F26" s="11">
         <v>13</v>
       </c>
@@ -2197,10 +2194,10 @@
       <c r="J26" s="6"/>
       <c r="K26" s="6"/>
       <c r="L26" s="6"/>
-      <c r="M26" s="15" t="s">
+      <c r="M26" s="49" t="s">
         <v>45</v>
       </c>
-      <c r="N26" s="15"/>
+      <c r="N26" s="49"/>
       <c r="P26" s="4">
         <v>11</v>
       </c>
@@ -2209,208 +2206,208 @@
       </c>
       <c r="R26" s="1"/>
       <c r="S26" s="1"/>
-      <c r="T26" s="36" t="s">
+      <c r="T26" s="60" t="s">
         <v>63</v>
       </c>
-      <c r="U26" s="37"/>
+      <c r="U26" s="61"/>
     </row>
     <row r="28" spans="1:21">
-      <c r="A28" s="20" t="s">
+      <c r="A28" s="74" t="s">
+        <v>80</v>
+      </c>
+      <c r="B28" s="74"/>
+      <c r="C28" s="74"/>
+      <c r="D28" s="74"/>
+      <c r="E28" s="74"/>
+      <c r="F28" s="74"/>
+      <c r="G28" s="74"/>
+      <c r="I28" s="73" t="s">
+        <v>70</v>
+      </c>
+      <c r="J28" s="73"/>
+      <c r="K28" s="73"/>
+      <c r="L28" s="73"/>
+      <c r="M28" s="73"/>
+      <c r="N28" s="73"/>
+      <c r="P28" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="29" spans="1:21">
+      <c r="A29" s="75" t="s">
+        <v>79</v>
+      </c>
+      <c r="B29" s="75"/>
+      <c r="C29" s="75"/>
+      <c r="D29" s="75"/>
+      <c r="E29" s="75"/>
+      <c r="F29" s="75"/>
+      <c r="G29" s="75"/>
+      <c r="I29" s="72" t="s">
         <v>81</v>
       </c>
-      <c r="B28" s="20"/>
-      <c r="C28" s="20"/>
-      <c r="D28" s="20"/>
-      <c r="E28" s="20"/>
-      <c r="F28" s="20"/>
-      <c r="G28" s="20"/>
-      <c r="I28" s="19" t="s">
-        <v>70</v>
-      </c>
-      <c r="J28" s="19"/>
-      <c r="K28" s="19"/>
-      <c r="L28" s="19"/>
-      <c r="M28" s="19"/>
-      <c r="N28" s="19"/>
-      <c r="P28" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="29" spans="1:21">
-      <c r="A29" s="21" t="s">
-        <v>80</v>
-      </c>
-      <c r="B29" s="21"/>
-      <c r="C29" s="21"/>
-      <c r="D29" s="21"/>
-      <c r="E29" s="21"/>
-      <c r="F29" s="21"/>
-      <c r="G29" s="21"/>
-      <c r="I29" s="18" t="s">
-        <v>82</v>
-      </c>
-      <c r="J29" s="19"/>
-      <c r="K29" s="19"/>
-      <c r="L29" s="19"/>
-      <c r="M29" s="19"/>
-      <c r="N29" s="19"/>
+      <c r="J29" s="73"/>
+      <c r="K29" s="73"/>
+      <c r="L29" s="73"/>
+      <c r="M29" s="73"/>
+      <c r="N29" s="73"/>
     </row>
     <row r="30" spans="1:21">
-      <c r="A30" s="22" t="s">
-        <v>92</v>
-      </c>
-      <c r="B30" s="22"/>
-      <c r="C30" s="22"/>
-      <c r="D30" s="22"/>
-      <c r="E30" s="22"/>
-      <c r="F30" s="22"/>
-      <c r="G30" s="22"/>
-      <c r="I30" s="19"/>
-      <c r="J30" s="19"/>
-      <c r="K30" s="19"/>
-      <c r="L30" s="19"/>
-      <c r="M30" s="19"/>
-      <c r="N30" s="19"/>
+      <c r="A30" s="76" t="s">
+        <v>91</v>
+      </c>
+      <c r="B30" s="76"/>
+      <c r="C30" s="76"/>
+      <c r="D30" s="76"/>
+      <c r="E30" s="76"/>
+      <c r="F30" s="76"/>
+      <c r="G30" s="76"/>
+      <c r="I30" s="73"/>
+      <c r="J30" s="73"/>
+      <c r="K30" s="73"/>
+      <c r="L30" s="73"/>
+      <c r="M30" s="73"/>
+      <c r="N30" s="73"/>
     </row>
     <row r="31" spans="1:21" ht="16" customHeight="1">
-      <c r="I31" s="23" t="s">
-        <v>97</v>
-      </c>
-      <c r="J31" s="23"/>
-      <c r="K31" s="23"/>
-      <c r="L31" s="23"/>
-      <c r="M31" s="23"/>
-      <c r="N31" s="23"/>
+      <c r="I31" s="77" t="s">
+        <v>96</v>
+      </c>
+      <c r="J31" s="77"/>
+      <c r="K31" s="77"/>
+      <c r="L31" s="77"/>
+      <c r="M31" s="77"/>
+      <c r="N31" s="77"/>
     </row>
     <row r="32" spans="1:21" ht="16" customHeight="1">
-      <c r="A32" s="71" t="s">
+      <c r="A32" s="19" t="s">
+        <v>98</v>
+      </c>
+      <c r="B32" s="20"/>
+      <c r="C32" s="20"/>
+      <c r="D32" s="20"/>
+      <c r="E32" s="20"/>
+      <c r="F32" s="20"/>
+      <c r="G32" s="21"/>
+      <c r="I32" s="77"/>
+      <c r="J32" s="77"/>
+      <c r="K32" s="77"/>
+      <c r="L32" s="77"/>
+      <c r="M32" s="77"/>
+      <c r="N32" s="77"/>
+    </row>
+    <row r="33" spans="1:14" ht="16" customHeight="1">
+      <c r="A33" s="22"/>
+      <c r="B33" s="23"/>
+      <c r="C33" s="23"/>
+      <c r="D33" s="23"/>
+      <c r="E33" s="23"/>
+      <c r="F33" s="23"/>
+      <c r="G33" s="24"/>
+      <c r="I33" s="77"/>
+      <c r="J33" s="77"/>
+      <c r="K33" s="77"/>
+      <c r="L33" s="77"/>
+      <c r="M33" s="77"/>
+      <c r="N33" s="77"/>
+    </row>
+    <row r="34" spans="1:14" ht="16" customHeight="1">
+      <c r="A34" s="22"/>
+      <c r="B34" s="23"/>
+      <c r="C34" s="23"/>
+      <c r="D34" s="23"/>
+      <c r="E34" s="23"/>
+      <c r="F34" s="23"/>
+      <c r="G34" s="24"/>
+      <c r="I34" s="77" t="s">
+        <v>83</v>
+      </c>
+      <c r="J34" s="77"/>
+      <c r="K34" s="77"/>
+      <c r="L34" s="77"/>
+      <c r="M34" s="77"/>
+      <c r="N34" s="77"/>
+    </row>
+    <row r="35" spans="1:14">
+      <c r="A35" s="22"/>
+      <c r="B35" s="23"/>
+      <c r="C35" s="23"/>
+      <c r="D35" s="23"/>
+      <c r="E35" s="23"/>
+      <c r="F35" s="23"/>
+      <c r="G35" s="24"/>
+      <c r="I35" s="77"/>
+      <c r="J35" s="77"/>
+      <c r="K35" s="77"/>
+      <c r="L35" s="77"/>
+      <c r="M35" s="77"/>
+      <c r="N35" s="77"/>
+    </row>
+    <row r="36" spans="1:14">
+      <c r="A36" s="22"/>
+      <c r="B36" s="23"/>
+      <c r="C36" s="23"/>
+      <c r="D36" s="23"/>
+      <c r="E36" s="23"/>
+      <c r="F36" s="23"/>
+      <c r="G36" s="24"/>
+      <c r="I36" s="73" t="s">
+        <v>93</v>
+      </c>
+      <c r="J36" s="73"/>
+      <c r="K36" s="73"/>
+      <c r="L36" s="73"/>
+      <c r="M36" s="73"/>
+      <c r="N36" s="73"/>
+    </row>
+    <row r="37" spans="1:14">
+      <c r="A37" s="22"/>
+      <c r="B37" s="23"/>
+      <c r="C37" s="23"/>
+      <c r="D37" s="23"/>
+      <c r="E37" s="23"/>
+      <c r="F37" s="23"/>
+      <c r="G37" s="24"/>
+      <c r="I37" s="72" t="s">
+        <v>95</v>
+      </c>
+      <c r="J37" s="72"/>
+      <c r="K37" s="72"/>
+      <c r="L37" s="72"/>
+      <c r="M37" s="72"/>
+      <c r="N37" s="72"/>
+    </row>
+    <row r="38" spans="1:14">
+      <c r="A38" s="22"/>
+      <c r="B38" s="23"/>
+      <c r="C38" s="23"/>
+      <c r="D38" s="23"/>
+      <c r="E38" s="23"/>
+      <c r="F38" s="23"/>
+      <c r="G38" s="24"/>
+      <c r="I38" s="72"/>
+      <c r="J38" s="72"/>
+      <c r="K38" s="72"/>
+      <c r="L38" s="72"/>
+      <c r="M38" s="72"/>
+      <c r="N38" s="72"/>
+    </row>
+    <row r="39" spans="1:14" ht="16" customHeight="1">
+      <c r="A39" s="25"/>
+      <c r="B39" s="26"/>
+      <c r="C39" s="26"/>
+      <c r="D39" s="26"/>
+      <c r="E39" s="26"/>
+      <c r="F39" s="26"/>
+      <c r="G39" s="27"/>
+      <c r="I39" s="16" t="s">
         <v>99</v>
       </c>
-      <c r="B32" s="69"/>
-      <c r="C32" s="69"/>
-      <c r="D32" s="69"/>
-      <c r="E32" s="69"/>
-      <c r="F32" s="69"/>
-      <c r="G32" s="72"/>
-      <c r="I32" s="23"/>
-      <c r="J32" s="23"/>
-      <c r="K32" s="23"/>
-      <c r="L32" s="23"/>
-      <c r="M32" s="23"/>
-      <c r="N32" s="23"/>
-    </row>
-    <row r="33" spans="1:14" ht="16" customHeight="1">
-      <c r="A33" s="73"/>
-      <c r="B33" s="70"/>
-      <c r="C33" s="70"/>
-      <c r="D33" s="70"/>
-      <c r="E33" s="70"/>
-      <c r="F33" s="70"/>
-      <c r="G33" s="74"/>
-      <c r="I33" s="23"/>
-      <c r="J33" s="23"/>
-      <c r="K33" s="23"/>
-      <c r="L33" s="23"/>
-      <c r="M33" s="23"/>
-      <c r="N33" s="23"/>
-    </row>
-    <row r="34" spans="1:14" ht="16" customHeight="1">
-      <c r="A34" s="73"/>
-      <c r="B34" s="70"/>
-      <c r="C34" s="70"/>
-      <c r="D34" s="70"/>
-      <c r="E34" s="70"/>
-      <c r="F34" s="70"/>
-      <c r="G34" s="74"/>
-      <c r="I34" s="23" t="s">
-        <v>84</v>
-      </c>
-      <c r="J34" s="23"/>
-      <c r="K34" s="23"/>
-      <c r="L34" s="23"/>
-      <c r="M34" s="23"/>
-      <c r="N34" s="23"/>
-    </row>
-    <row r="35" spans="1:14">
-      <c r="A35" s="73"/>
-      <c r="B35" s="70"/>
-      <c r="C35" s="70"/>
-      <c r="D35" s="70"/>
-      <c r="E35" s="70"/>
-      <c r="F35" s="70"/>
-      <c r="G35" s="74"/>
-      <c r="I35" s="23"/>
-      <c r="J35" s="23"/>
-      <c r="K35" s="23"/>
-      <c r="L35" s="23"/>
-      <c r="M35" s="23"/>
-      <c r="N35" s="23"/>
-    </row>
-    <row r="36" spans="1:14">
-      <c r="A36" s="73"/>
-      <c r="B36" s="70"/>
-      <c r="C36" s="70"/>
-      <c r="D36" s="70"/>
-      <c r="E36" s="70"/>
-      <c r="F36" s="70"/>
-      <c r="G36" s="74"/>
-      <c r="I36" s="19" t="s">
-        <v>94</v>
-      </c>
-      <c r="J36" s="19"/>
-      <c r="K36" s="19"/>
-      <c r="L36" s="19"/>
-      <c r="M36" s="19"/>
-      <c r="N36" s="19"/>
-    </row>
-    <row r="37" spans="1:14">
-      <c r="A37" s="73"/>
-      <c r="B37" s="70"/>
-      <c r="C37" s="70"/>
-      <c r="D37" s="70"/>
-      <c r="E37" s="70"/>
-      <c r="F37" s="70"/>
-      <c r="G37" s="74"/>
-      <c r="I37" s="18" t="s">
-        <v>96</v>
-      </c>
-      <c r="J37" s="18"/>
-      <c r="K37" s="18"/>
-      <c r="L37" s="18"/>
-      <c r="M37" s="18"/>
-      <c r="N37" s="18"/>
-    </row>
-    <row r="38" spans="1:14">
-      <c r="A38" s="73"/>
-      <c r="B38" s="70"/>
-      <c r="C38" s="70"/>
-      <c r="D38" s="70"/>
-      <c r="E38" s="70"/>
-      <c r="F38" s="70"/>
-      <c r="G38" s="74"/>
-      <c r="I38" s="18"/>
-      <c r="J38" s="18"/>
-      <c r="K38" s="18"/>
-      <c r="L38" s="18"/>
-      <c r="M38" s="18"/>
-      <c r="N38" s="18"/>
-    </row>
-    <row r="39" spans="1:14" ht="16" customHeight="1">
-      <c r="A39" s="75"/>
-      <c r="B39" s="76"/>
-      <c r="C39" s="76"/>
-      <c r="D39" s="76"/>
-      <c r="E39" s="76"/>
-      <c r="F39" s="76"/>
-      <c r="G39" s="77"/>
-      <c r="I39" s="66" t="s">
-        <v>100</v>
-      </c>
-      <c r="J39" s="67"/>
-      <c r="K39" s="67"/>
-      <c r="L39" s="67"/>
-      <c r="M39" s="67"/>
-      <c r="N39" s="68"/>
+      <c r="J39" s="17"/>
+      <c r="K39" s="17"/>
+      <c r="L39" s="17"/>
+      <c r="M39" s="17"/>
+      <c r="N39" s="18"/>
     </row>
     <row r="40" spans="1:14">
       <c r="A40" s="13"/>
@@ -2420,12 +2417,12 @@
       <c r="E40" s="13"/>
       <c r="F40" s="13"/>
       <c r="G40" s="13"/>
-      <c r="I40" s="65"/>
-      <c r="J40" s="65"/>
-      <c r="K40" s="65"/>
-      <c r="L40" s="65"/>
-      <c r="M40" s="65"/>
-      <c r="N40" s="65"/>
+      <c r="I40" s="15"/>
+      <c r="J40" s="15"/>
+      <c r="K40" s="15"/>
+      <c r="L40" s="15"/>
+      <c r="M40" s="15"/>
+      <c r="N40" s="15"/>
     </row>
     <row r="41" spans="1:14">
       <c r="A41" s="13"/>
@@ -2441,16 +2438,55 @@
     </row>
   </sheetData>
   <mergeCells count="81">
-    <mergeCell ref="I39:N39"/>
-    <mergeCell ref="A32:G39"/>
-    <mergeCell ref="M21:N21"/>
-    <mergeCell ref="M20:N20"/>
-    <mergeCell ref="I14:I19"/>
-    <mergeCell ref="K14:K16"/>
-    <mergeCell ref="N15:N16"/>
-    <mergeCell ref="K17:K19"/>
-    <mergeCell ref="N18:N19"/>
-    <mergeCell ref="J14:J19"/>
+    <mergeCell ref="A30:G30"/>
+    <mergeCell ref="I28:N28"/>
+    <mergeCell ref="I29:N30"/>
+    <mergeCell ref="I31:N33"/>
+    <mergeCell ref="I34:N35"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="A4:A19"/>
+    <mergeCell ref="B4:B21"/>
+    <mergeCell ref="C4:C26"/>
+    <mergeCell ref="D4:D26"/>
+    <mergeCell ref="A20:A26"/>
+    <mergeCell ref="B22:B26"/>
+    <mergeCell ref="E24:E26"/>
+    <mergeCell ref="T24:U24"/>
+    <mergeCell ref="M24:N24"/>
+    <mergeCell ref="T25:U25"/>
+    <mergeCell ref="T26:U26"/>
+    <mergeCell ref="M25:N25"/>
+    <mergeCell ref="M26:N26"/>
+    <mergeCell ref="T21:U21"/>
+    <mergeCell ref="T20:U20"/>
+    <mergeCell ref="T22:U22"/>
+    <mergeCell ref="T23:U23"/>
+    <mergeCell ref="E4:E20"/>
+    <mergeCell ref="E21:E22"/>
+    <mergeCell ref="P14:P19"/>
+    <mergeCell ref="Q14:Q19"/>
+    <mergeCell ref="R14:R16"/>
+    <mergeCell ref="U15:U16"/>
+    <mergeCell ref="R17:R19"/>
+    <mergeCell ref="U18:U19"/>
+    <mergeCell ref="T6:U6"/>
+    <mergeCell ref="T7:U7"/>
+    <mergeCell ref="P8:P13"/>
+    <mergeCell ref="Q8:Q13"/>
+    <mergeCell ref="R8:R10"/>
+    <mergeCell ref="U9:U10"/>
+    <mergeCell ref="R11:R13"/>
+    <mergeCell ref="U12:U13"/>
+    <mergeCell ref="G14:G19"/>
+    <mergeCell ref="N9:N10"/>
+    <mergeCell ref="N12:N13"/>
+    <mergeCell ref="P1:U1"/>
+    <mergeCell ref="P2:S2"/>
+    <mergeCell ref="T2:U2"/>
+    <mergeCell ref="T4:U4"/>
+    <mergeCell ref="T5:U5"/>
     <mergeCell ref="I1:N1"/>
     <mergeCell ref="F2:F3"/>
     <mergeCell ref="G2:G3"/>
@@ -2467,61 +2503,22 @@
     <mergeCell ref="I8:I13"/>
     <mergeCell ref="K8:K10"/>
     <mergeCell ref="K11:K13"/>
-    <mergeCell ref="P1:U1"/>
-    <mergeCell ref="P2:S2"/>
-    <mergeCell ref="T2:U2"/>
-    <mergeCell ref="T4:U4"/>
-    <mergeCell ref="T5:U5"/>
-    <mergeCell ref="R8:R10"/>
-    <mergeCell ref="U9:U10"/>
-    <mergeCell ref="R11:R13"/>
-    <mergeCell ref="U12:U13"/>
-    <mergeCell ref="G14:G19"/>
-    <mergeCell ref="N9:N10"/>
-    <mergeCell ref="N12:N13"/>
-    <mergeCell ref="T21:U21"/>
-    <mergeCell ref="T20:U20"/>
-    <mergeCell ref="T22:U22"/>
-    <mergeCell ref="T23:U23"/>
-    <mergeCell ref="E4:E20"/>
-    <mergeCell ref="E21:E22"/>
-    <mergeCell ref="P14:P19"/>
-    <mergeCell ref="Q14:Q19"/>
-    <mergeCell ref="R14:R16"/>
-    <mergeCell ref="U15:U16"/>
-    <mergeCell ref="R17:R19"/>
-    <mergeCell ref="U18:U19"/>
-    <mergeCell ref="T6:U6"/>
-    <mergeCell ref="T7:U7"/>
-    <mergeCell ref="P8:P13"/>
-    <mergeCell ref="Q8:Q13"/>
-    <mergeCell ref="T24:U24"/>
-    <mergeCell ref="M24:N24"/>
-    <mergeCell ref="T25:U25"/>
-    <mergeCell ref="T26:U26"/>
-    <mergeCell ref="M25:N25"/>
-    <mergeCell ref="M26:N26"/>
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="A2:D2"/>
-    <mergeCell ref="A1:G1"/>
-    <mergeCell ref="A4:A19"/>
-    <mergeCell ref="B4:B21"/>
-    <mergeCell ref="C4:C26"/>
-    <mergeCell ref="D4:D26"/>
-    <mergeCell ref="A20:A26"/>
-    <mergeCell ref="B22:B26"/>
-    <mergeCell ref="E24:E26"/>
+    <mergeCell ref="I39:N39"/>
+    <mergeCell ref="A32:G39"/>
+    <mergeCell ref="M21:N21"/>
+    <mergeCell ref="M20:N20"/>
+    <mergeCell ref="I14:I19"/>
+    <mergeCell ref="K14:K16"/>
+    <mergeCell ref="N15:N16"/>
+    <mergeCell ref="K17:K19"/>
+    <mergeCell ref="N18:N19"/>
+    <mergeCell ref="J14:J19"/>
     <mergeCell ref="M23:N23"/>
     <mergeCell ref="M22:N22"/>
     <mergeCell ref="I37:N38"/>
     <mergeCell ref="I36:N36"/>
     <mergeCell ref="A28:G28"/>
     <mergeCell ref="A29:G29"/>
-    <mergeCell ref="A30:G30"/>
-    <mergeCell ref="I28:N28"/>
-    <mergeCell ref="I29:N30"/>
-    <mergeCell ref="I31:N33"/>
-    <mergeCell ref="I34:N35"/>
   </mergeCells>
   <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="59" fitToHeight="0" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>